<commit_message>
Updated data model with changes discussed with Rob and Siva
</commit_message>
<xml_diff>
--- a/docs/BC Parks CMS Data Model.xlsx
+++ b/docs/BC Parks CMS Data Model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\177012\Documents\BC Parks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\177150\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD59D07D-4C14-4D1B-8756-A6528DC8A2E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCECDFA0-47AF-4EFF-B983-B915B95C4DF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A33082D8-1C98-4870-8924-9924FABEACC5}"/>
+    <workbookView xWindow="4740" yWindow="1080" windowWidth="21600" windowHeight="11385" xr2:uid="{A33082D8-1C98-4870-8924-9924FABEACC5}"/>
   </bookViews>
   <sheets>
     <sheet name="BCParks" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="114">
   <si>
     <t>Table</t>
   </si>
@@ -165,9 +165,6 @@
     <t>RepealedDate</t>
   </si>
   <si>
-    <t>Active</t>
-  </si>
-  <si>
     <t>MarineProtectedArea</t>
   </si>
   <si>
@@ -252,9 +249,6 @@
     <t>All in One table</t>
   </si>
   <si>
-    <t>Coordinates</t>
-  </si>
-  <si>
     <t>Link to PAR Data</t>
   </si>
   <si>
@@ -303,9 +297,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Should this be in one field, or should it be separated to Latitude/Longitude (digital lat/long)?</t>
-  </si>
-  <si>
     <t>Used to estimate an end date; the status should be assessed before this date; equivalent to rescinded date if it's a closure</t>
   </si>
   <si>
@@ -361,13 +352,37 @@
   </si>
   <si>
     <t>Link to EventType</t>
+  </si>
+  <si>
+    <t>Values will be -  open,full closure,partial closure,inaccessible,warning,restricted,permit required,closed to the public</t>
+  </si>
+  <si>
+    <t>Director's Order, Map,Evacuation, Information Bulletin</t>
+  </si>
+  <si>
+    <t>Link to ManagementArea</t>
+  </si>
+  <si>
+    <t>Link to Protected Area or Site</t>
+  </si>
+  <si>
+    <t>ManagementAreaNumber</t>
+  </si>
+  <si>
+    <t>SectionNumber</t>
+  </si>
+  <si>
+    <t>RegionNumber</t>
+  </si>
+  <si>
+    <t>EventID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,6 +431,12 @@
     <font>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -542,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -567,9 +588,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -582,6 +600,14 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -896,11 +922,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9256A4-85B0-483D-ABA5-01E16592AE65}">
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:G104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -927,38 +953,38 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
     </row>
     <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>98</v>
+      <c r="C3" s="22" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>99</v>
+      <c r="C4" s="21" t="s">
+        <v>96</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>23</v>
@@ -966,11 +992,11 @@
     </row>
     <row r="5" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>99</v>
+      <c r="C5" s="21" t="s">
+        <v>96</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>22</v>
@@ -978,35 +1004,35 @@
     </row>
     <row r="6" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>90</v>
+      <c r="C6" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>99</v>
+      <c r="C7" s="21" t="s">
+        <v>96</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>99</v>
+      <c r="C8" s="21" t="s">
+        <v>96</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>24</v>
@@ -1014,11 +1040,11 @@
     </row>
     <row r="9" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>99</v>
+      <c r="C9" s="21" t="s">
+        <v>96</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>21</v>
@@ -1026,10 +1052,10 @@
     </row>
     <row r="10" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
-      <c r="B10" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="22"/>
+      <c r="B10" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="21"/>
       <c r="D10" s="7" t="s">
         <v>26</v>
       </c>
@@ -1037,127 +1063,129 @@
     </row>
     <row r="11" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>99</v>
+      <c r="C11" s="21" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>99</v>
+      <c r="C12" s="21" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="22" t="s">
-        <v>99</v>
+      <c r="C13" s="21" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="22" t="s">
-        <v>100</v>
+      <c r="C14" s="21" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
-      <c r="B17" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>98</v>
+      <c r="B17" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
-      <c r="B18" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="22"/>
+      <c r="B18" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>109</v>
+      </c>
       <c r="D18" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="22" t="s">
-        <v>100</v>
+      <c r="C19" s="21" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="22" t="s">
-        <v>100</v>
+      <c r="C20" s="21" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
-      <c r="B21" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>100</v>
+      <c r="B21" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="32" t="s">
-        <v>107</v>
+      <c r="C22" s="31" t="s">
+        <v>104</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="32" t="s">
-        <v>108</v>
+      <c r="C23" s="31" t="s">
+        <v>105</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="22" t="s">
-        <v>98</v>
+      <c r="C24" s="21" t="s">
+        <v>95</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>38</v>
@@ -1165,71 +1193,71 @@
     </row>
     <row r="25" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
-      <c r="B25" s="24" t="s">
-        <v>95</v>
+      <c r="B25" s="23" t="s">
+        <v>92</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
-      <c r="B26" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>100</v>
+      <c r="B26" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
-      <c r="B27" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="31" t="s">
-        <v>100</v>
+      <c r="B27" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
-      <c r="B28" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>100</v>
+      <c r="B28" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
-      <c r="B29" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>100</v>
+      <c r="B29" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
-      <c r="B30" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="32" t="s">
-        <v>106</v>
+      <c r="B30" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>103</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="31" t="s">
-        <v>100</v>
+      <c r="C31" s="30" t="s">
+        <v>97</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>34</v>
@@ -1237,11 +1265,11 @@
     </row>
     <row r="32" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="31" t="s">
-        <v>100</v>
+      <c r="C32" s="30" t="s">
+        <v>97</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>35</v>
@@ -1249,26 +1277,26 @@
     </row>
     <row r="33" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="31" t="s">
-        <v>100</v>
+      <c r="C33" s="30" t="s">
+        <v>97</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="31" t="s">
-        <v>98</v>
+      <c r="C34" s="30" t="s">
+        <v>95</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>37</v>
@@ -1276,11 +1304,11 @@
     </row>
     <row r="35" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="31" t="s">
-        <v>100</v>
+      <c r="C35" s="30" t="s">
+        <v>97</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>25</v>
@@ -1288,68 +1316,68 @@
     </row>
     <row r="36" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5"/>
-      <c r="B36" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" s="22"/>
-      <c r="G36" s="19" t="s">
-        <v>89</v>
-      </c>
+      <c r="B36" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="G36" s="19"/>
     </row>
     <row r="37" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5"/>
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="22" t="s">
-        <v>102</v>
+      <c r="C37" s="21" t="s">
+        <v>99</v>
       </c>
       <c r="G37" s="19"/>
     </row>
     <row r="38" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="22" t="s">
-        <v>102</v>
+      <c r="C38" s="21" t="s">
+        <v>99</v>
       </c>
       <c r="G38" s="19"/>
     </row>
     <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5"/>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="22" t="s">
-        <v>99</v>
+      <c r="C39" s="21" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5"/>
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="22" t="s">
-        <v>100</v>
+      <c r="C40" s="21" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="22" t="s">
-        <v>99</v>
+      <c r="C41" s="21" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="9"/>
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="22" t="s">
-        <v>100</v>
+      <c r="C42" s="21" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -1376,99 +1404,105 @@
       </c>
     </row>
     <row r="49" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="30" t="s">
+      <c r="A49" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="28"/>
-      <c r="C49" s="28"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
     </row>
     <row r="50" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5"/>
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C50" s="22" t="s">
-        <v>100</v>
+      <c r="C50" s="21" t="s">
+        <v>97</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5"/>
     </row>
-    <row r="52" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="27" t="s">
+    <row r="52" spans="1:6" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A52" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B52" s="28"/>
-      <c r="C52" s="28"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="34" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="53" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="21"/>
-      <c r="B53" s="22" t="s">
+      <c r="A53" s="20"/>
+      <c r="B53" s="21" t="s">
         <v>29</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E53" s="19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5"/>
     </row>
     <row r="55" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="B55" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="C55" s="28" t="s">
+      <c r="A55" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C55" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="D55" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
     </row>
     <row r="57" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="B57" s="28" t="s">
+      <c r="A57" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B57" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C57" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="D57" s="27"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="28"/>
+      <c r="C57" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="D57" s="26"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="21"/>
-      <c r="B58" s="22" t="s">
-        <v>54</v>
+      <c r="A58" s="20"/>
+      <c r="B58" s="21" t="s">
+        <v>53</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>100</v>
+        <v>97</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="21"/>
-      <c r="B59" s="22" t="s">
-        <v>45</v>
+      <c r="A59" s="20"/>
+      <c r="B59" s="21" t="s">
+        <v>44</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -1477,307 +1511,323 @@
       <c r="C60" s="6"/>
     </row>
     <row r="61" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="27" t="s">
+      <c r="A61" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B61" s="28"/>
-      <c r="C61" s="28"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="27"/>
       <c r="D61" s="11"/>
       <c r="E61" s="18"/>
       <c r="F61" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="5"/>
-      <c r="B62" s="23" t="s">
+      <c r="B62" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C62" s="23"/>
+      <c r="C62" s="22"/>
     </row>
     <row r="63" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="5"/>
-      <c r="B63" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="C63" s="22"/>
+      <c r="B63" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C63" s="21"/>
       <c r="D63" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="64" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="5"/>
-      <c r="B64" s="22" t="s">
+      <c r="B64" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C64" s="22"/>
+      <c r="C64" s="21"/>
     </row>
     <row r="65" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="5"/>
-      <c r="B65" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="C65" s="22"/>
+      <c r="B65" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C65" s="21"/>
     </row>
     <row r="66" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="5"/>
-      <c r="B66" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="C66" s="29"/>
+      <c r="B66" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="C66" s="28"/>
     </row>
     <row r="67" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="5"/>
-      <c r="B67" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C67" s="22"/>
+      <c r="B67" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C67" s="21"/>
     </row>
     <row r="68" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="5"/>
-      <c r="B68" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C68" s="22"/>
+      <c r="B68" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C68" s="21"/>
       <c r="D68" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="69" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="5"/>
-      <c r="B69" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C69" s="22"/>
+      <c r="B69" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C69" s="21"/>
     </row>
     <row r="70" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="5"/>
-      <c r="B70" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C70" s="22"/>
+      <c r="B70" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C70" s="21"/>
     </row>
     <row r="71" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="5"/>
-      <c r="B71" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C71" s="22"/>
+      <c r="B71" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C71" s="21"/>
     </row>
     <row r="72" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="5"/>
-      <c r="B72" s="22" t="s">
+      <c r="B72" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C72" s="22"/>
+      <c r="C72" s="21"/>
     </row>
     <row r="73" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="5"/>
-      <c r="B73" s="22" t="s">
+      <c r="B73" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C73" s="22"/>
+      <c r="C73" s="21"/>
     </row>
     <row r="74" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="5"/>
-      <c r="B74" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C74" s="22"/>
+      <c r="B74" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C74" s="21"/>
     </row>
     <row r="75" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="5"/>
-      <c r="B75" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C75" s="22"/>
+      <c r="B75" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C75" s="21"/>
     </row>
     <row r="76" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="5"/>
-      <c r="B76" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C76" s="22"/>
+      <c r="B76" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C76" s="21"/>
     </row>
     <row r="77" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="5"/>
-      <c r="B77" s="22" t="s">
+      <c r="B77" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C77" s="21"/>
+    </row>
+    <row r="78" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="5"/>
+      <c r="B78" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C77" s="22"/>
-    </row>
-    <row r="78" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="9"/>
-      <c r="B78" s="22" t="s">
+      <c r="C78" s="21"/>
+    </row>
+    <row r="79" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="5"/>
+      <c r="B79" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C79" s="31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="9"/>
+      <c r="B80" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C80" s="31" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="C78" s="22"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B80" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C80" s="28"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B81" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C81" s="23"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="4"/>
-      <c r="B82" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C82" s="22"/>
+      <c r="B82" s="27"/>
+      <c r="C82" s="27"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B83" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C83" s="22"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" s="4"/>
+      <c r="B84" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C84" s="21"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B85" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C85" s="21"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B86" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C86" s="21"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B87" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C87" s="21"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B88" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C83" s="22"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B84" s="22" t="s">
+      <c r="C88" s="21"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B89" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C89" s="21"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B90" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C90" s="21"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B91" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C91" s="21"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B92" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C92" s="21"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B93" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C93" s="21"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B95" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C95" s="27"/>
+      <c r="F95" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G95" s="32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B96" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C96" s="22"/>
+      <c r="G96" s="32"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B97" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C84" s="22"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B85" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C85" s="22"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B86" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C86" s="22"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B87" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="C87" s="22"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B88" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C88" s="22"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B89" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C89" s="22"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B90" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C90" s="22"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B91" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C91" s="22"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" s="27" t="s">
+      <c r="C97" s="21"/>
+      <c r="D97" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G97" s="32"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G98" s="32"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B93" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C93" s="28"/>
-      <c r="F93" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G93" s="20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B94" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C94" s="23"/>
-      <c r="G94" s="20"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B95" s="22" t="s">
+      <c r="B99" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="C99" s="27"/>
+      <c r="F99" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G99" s="32"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B100" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C100" s="22"/>
+      <c r="G100" s="32"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B101" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C95" s="22"/>
-      <c r="D95" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G95" s="20"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G96" s="20"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" s="27" t="s">
+      <c r="C101" s="21"/>
+      <c r="D101" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G101" s="32"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F102" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G102" s="32"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B97" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C97" s="28"/>
-      <c r="F97" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G97" s="20"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B98" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C98" s="23"/>
-      <c r="G98" s="20"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B99" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C99" s="22"/>
-      <c r="D99" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G99" s="20"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F100" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G100" s="20"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="B101" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C101" s="28"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B102" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C102" s="23"/>
+      <c r="B103" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C103" s="27"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B104" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C104" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G93:G100"/>
+    <mergeCell ref="G95:G102"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
load fire zone references to park
</commit_message>
<xml_diff>
--- a/docs/BC Parks CMS Data Model.xlsx
+++ b/docs/BC Parks CMS Data Model.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\177012\Documents\BC Parks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub\BCP-CMS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{003AE97F-B474-4854-A4B4-6C59A1948941}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{15DC0B95-9021-445E-90BC-E0F067095CBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="3090" windowWidth="21600" windowHeight="11385" xr2:uid="{A33082D8-1C98-4870-8924-9924FABEACC5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A33082D8-1C98-4870-8924-9924FABEACC5}"/>
   </bookViews>
   <sheets>
     <sheet name="BCParks" sheetId="1" r:id="rId1"/>
-    <sheet name="BCParks - old" sheetId="3" r:id="rId2"/>
-    <sheet name="BCGNIS" sheetId="2" r:id="rId3"/>
+    <sheet name="DataCatalogue" sheetId="4" r:id="rId2"/>
+    <sheet name="Datasets" sheetId="5" r:id="rId3"/>
+    <sheet name="BCGNIS" sheetId="2" r:id="rId4"/>
+    <sheet name="BCParks - old" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="350">
   <si>
     <t>Table</t>
   </si>
@@ -385,18 +387,12 @@
     <t>Moved to Links[]</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Link to AdvisoryStatus</t>
   </si>
   <si>
     <t>boolean</t>
   </si>
   <si>
-    <t>x - deleted field</t>
-  </si>
-  <si>
     <t>Public Advisory History</t>
   </si>
   <si>
@@ -436,15 +432,6 @@
     <t>removed spaces to match standard field name format</t>
   </si>
   <si>
-    <t>changed to upper-case U for consistency</t>
-  </si>
-  <si>
-    <t>Start date of the event</t>
-  </si>
-  <si>
-    <t>Also referred to as 'PostDate'; used to schedule the start date and to display the date the advisory was posted; this is not necessarily the date the record was created and is not necessarily the event start date.</t>
-  </si>
-  <si>
     <t>Regions[]</t>
   </si>
   <si>
@@ -461,13 +448,1310 @@
   </si>
   <si>
     <t>Used to apply the advisory to management area(s)</t>
+  </si>
+  <si>
+    <t>DisplayAdvisoryDate</t>
+  </si>
+  <si>
+    <t>Used to enable/disable the display of the AdvisoryDate</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>Draft</t>
+  </si>
+  <si>
+    <t>Approval Requested</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Advisory is expired and has been removed from public display, but the record is not deleted.</t>
+  </si>
+  <si>
+    <t>Advisory saved as a draft by the user and is still in progress; not ready to submit for approval. Other staff may access it and collaborate on the content.</t>
+  </si>
+  <si>
+    <t>Draft has been saved and submitted to the web team for approval.  Approvers could also be select management staff in case of emergency situations.</t>
+  </si>
+  <si>
+    <t>Advisory approved to be published, but the publish action may or may not need to be scheduled for a specific date and time.  The preset PostedDate (AdvisoryDate) will control the date and time that it will be published.</t>
+  </si>
+  <si>
+    <t>Also referred to as 'PostDate'; used to schedule the publish date and to display the date the advisory was posted; this is not necessarily the date the record was created and is not necessarily the event start date</t>
+  </si>
+  <si>
+    <t>Start date of the event, also referred to as 'StartDate'</t>
+  </si>
+  <si>
+    <t>DisplayEndDate</t>
+  </si>
+  <si>
+    <t>Used to enable/disable the display of the EndDate</t>
+  </si>
+  <si>
+    <t>DisplayEffectiveDate</t>
+  </si>
+  <si>
+    <t>Used to enable/disable the display of the EffectiveDate (StartDate)</t>
+  </si>
+  <si>
+    <t>DisplayUpdatedDate</t>
+  </si>
+  <si>
+    <t>Used to enable/disable the display of the UpdatedDate</t>
+  </si>
+  <si>
+    <t>Indicates that the site record is a custom entry that does not exist in PAR</t>
+  </si>
+  <si>
+    <t>Administrative note, likely used to explain the purpose of the custom site entry</t>
+  </si>
+  <si>
+    <t>Advisory has been published and is publicly accessible via API.</t>
+  </si>
+  <si>
+    <t>FireCentre</t>
+  </si>
+  <si>
+    <t>FireCentreNumber</t>
+  </si>
+  <si>
+    <t>FireCentreName</t>
+  </si>
+  <si>
+    <t>FireZone</t>
+  </si>
+  <si>
+    <t>FireZoneNumber</t>
+  </si>
+  <si>
+    <t>FireZoneName</t>
+  </si>
+  <si>
+    <t>FireZones[]</t>
+  </si>
+  <si>
+    <t>HeadquartersCityName</t>
+  </si>
+  <si>
+    <t>Layer Display Name</t>
+  </si>
+  <si>
+    <t>Data Catalogue URL</t>
+  </si>
+  <si>
+    <t>Layer Reference</t>
+  </si>
+  <si>
+    <t>BC Parks, Ecological Reserves, and Protected Areas</t>
+  </si>
+  <si>
+    <t>https://openmaps.gov.bc.ca/geo/pub/WHSE_TANTALIS.TA_PARK_ECORES_PA_SVW/ows?service=WMS&amp;request=GetCapabilities</t>
+  </si>
+  <si>
+    <t>https://catalogue.data.gov.bc.ca/dataset/bc-parks-ecological-reserves-and-protected-areas</t>
+  </si>
+  <si>
+    <t>WHSE_TANTALIS.TA_PARK_ECORES_PA_SVW</t>
+  </si>
+  <si>
+    <t>TANTALIS - Conservancy Areas</t>
+  </si>
+  <si>
+    <t>BC Parks Conservancy Areas</t>
+  </si>
+  <si>
+    <t>https://openmaps.gov.bc.ca/geo/pub/WHSE_TANTALIS.TA_CONSERVANCY_AREAS_SVW/ows?service=WMS&amp;request=GetCapabilities</t>
+  </si>
+  <si>
+    <t>https://catalogue.data.gov.bc.ca/dataset/tantalis-conservancy-areas</t>
+  </si>
+  <si>
+    <t>WHSE_TANTALIS.TA_CONSERVANCY_AREAS_SVW</t>
+  </si>
+  <si>
+    <t>Parks and Protected Areas Regional Boundaries</t>
+  </si>
+  <si>
+    <t>BC Parks Regional Boundaries</t>
+  </si>
+  <si>
+    <t>https://openmaps.gov.bc.ca/geo/pub/WHSE_ADMIN_BOUNDARIES.ADM_BC_PARKS_REGIONS_SP/ows?service=WMS&amp;request=GetCapabilities</t>
+  </si>
+  <si>
+    <t>https://catalogue.data.gov.bc.ca/dataset/parks-and-protected-areas-regional-boundaries</t>
+  </si>
+  <si>
+    <t>WHSE_ADMIN_BOUNDARIES.ADM_BC_PARKS_REGIONS_SP</t>
+  </si>
+  <si>
+    <t>Parks and Protected Areas Section Boundaries</t>
+  </si>
+  <si>
+    <t>BC Parks Section Boundaries</t>
+  </si>
+  <si>
+    <t>https://openmaps.gov.bc.ca/geo/pub/WHSE_ADMIN_BOUNDARIES.ADM_BC_PARKS_SECTIONS_SP/ows?service=WMS&amp;request=GetCapabilities</t>
+  </si>
+  <si>
+    <t>https://catalogue.data.gov.bc.ca/dataset/parks-and-protected-areas-section-boundaries</t>
+  </si>
+  <si>
+    <t>WHSE_ADMIN_BOUNDARIES.ADM_BC_PARKS_SECTIONS_SP</t>
+  </si>
+  <si>
+    <t>Fire Centres</t>
+  </si>
+  <si>
+    <t>https://openmaps.gov.bc.ca/geo/pub/WHSE_LEGAL_ADMIN_BOUNDARIES.DRP_MOF_FIRE_CENTRES_SP/ows?service=WMS&amp;request=GetCapabilities</t>
+  </si>
+  <si>
+    <t>WHSE_LEGAL_ADMIN_BOUNDARIES.DRP_MOF_FIRE_CENTRES_SP</t>
+  </si>
+  <si>
+    <t>Fire Zones</t>
+  </si>
+  <si>
+    <t>https://openmaps.gov.bc.ca/geo/pub/WHSE_LEGAL_ADMIN_BOUNDARIES.DRP_MOF_FIRE_ZONES_SP/ows?service=WMS&amp;request=GetCapabilities</t>
+  </si>
+  <si>
+    <t>WHSE_LEGAL_ADMIN_BOUNDARIES.DRP_MOF_FIRE_ZONES_SP</t>
+  </si>
+  <si>
+    <t>Protected Lands Access Restrictions</t>
+  </si>
+  <si>
+    <t>https://openmaps.gov.bc.ca/geo/pub/WHSE_PARKS.PA_PRTCTD_LND_RSTRCTNS_SV/ows?service=WMS&amp;request=GetCapabilities</t>
+  </si>
+  <si>
+    <t>https://catalogue.data.gov.bc.ca/dataset/protected-lands-access-restrictions</t>
+  </si>
+  <si>
+    <t>WHSE_PARKS.PA_PRTCTD_LND_RSTRCTNS_SV</t>
+  </si>
+  <si>
+    <t>Protected Lands Facilities</t>
+  </si>
+  <si>
+    <t>https://openmaps.gov.bc.ca/geo/pub/WHSE_PARKS.PA_PRTCTD_LND_FACILITIES_SP/ows?service=WMS&amp;request=GetCapabilities</t>
+  </si>
+  <si>
+    <t>https://catalogue.data.gov.bc.ca/dataset/protected-lands-facilities</t>
+  </si>
+  <si>
+    <t>WHSE_PARKS.PA_PRTCTD_LND_FACILITIES_SP</t>
+  </si>
+  <si>
+    <t>This is not yet used</t>
+  </si>
+  <si>
+    <t>Emergency Management BC Boundaries</t>
+  </si>
+  <si>
+    <t>https://openmaps.gov.bc.ca/geo/pub/WHSE_LEGAL_ADMIN_BOUNDARIES.DRP_PEP_REGIONS_SP/ows?service=WMS&amp;request=GetCapabilities</t>
+  </si>
+  <si>
+    <t>https://catalogue.data.gov.bc.ca/dataset/emergency-management-bc-boundaries</t>
+  </si>
+  <si>
+    <t>WHSE_LEGAL_ADMIN_BOUNDARIES.DRP_PEP_REGIONS_SP</t>
+  </si>
+  <si>
+    <t>Natural Resource (NR) Areas</t>
+  </si>
+  <si>
+    <t>https://openmaps.gov.bc.ca/geo/pub/WHSE_ADMIN_BOUNDARIES.ADM_NR_AREAS_SPG/ows?service=WMS&amp;request=GetCapabilities</t>
+  </si>
+  <si>
+    <t>https://catalogue.data.gov.bc.ca/dataset/natural-resource-nr-areas</t>
+  </si>
+  <si>
+    <t>WHSE_ADMIN_BOUNDARIES.ADM_NR_AREAS_SPG</t>
+  </si>
+  <si>
+    <t>Natural Resource (NR) Regions</t>
+  </si>
+  <si>
+    <t>https://openmaps.gov.bc.ca/geo/pub/WHSE_ADMIN_BOUNDARIES.ADM_NR_REGIONS_SPG/ows?service=WMS&amp;request=GetCapabilities</t>
+  </si>
+  <si>
+    <t>https://catalogue.data.gov.bc.ca/dataset/natural-resource-nr-regions</t>
+  </si>
+  <si>
+    <t>WHSE_ADMIN_BOUNDARIES.ADM_NR_REGIONS_SPG</t>
+  </si>
+  <si>
+    <t>Natural Resource (NR) Districts</t>
+  </si>
+  <si>
+    <t>https://openmaps.gov.bc.ca/geo/pub/WHSE_ADMIN_BOUNDARIES.ADM_NR_DISTRICTS_SPG/ows?service=WMS&amp;request=GetCapabilities</t>
+  </si>
+  <si>
+    <t>https://catalogue.data.gov.bc.ca/dataset/natural-resource-nr-district</t>
+  </si>
+  <si>
+    <t>WHSE_ADMIN_BOUNDARIES.ADM_NR_DISTRICTS_SPG</t>
+  </si>
+  <si>
+    <t>BC Tourism Regions</t>
+  </si>
+  <si>
+    <t>https://openmaps.gov.bc.ca/geo/pub/WHSE_LEGAL_ADMIN_BOUNDARIES.ADM_TOURISM_REGIONS_SP/ows?service=WMS&amp;request=GetCapabilities</t>
+  </si>
+  <si>
+    <t>https://catalogue.data.gov.bc.ca/dataset/bc-tourism-regions</t>
+  </si>
+  <si>
+    <t>WHSE_LEGAL_ADMIN_BOUNDARIES.ADM_TOURISM_REGIONS_SP</t>
+  </si>
+  <si>
+    <t>Regional Districts - Legally Defined Administrative Areas of BC</t>
+  </si>
+  <si>
+    <t>BC Regional Districts</t>
+  </si>
+  <si>
+    <t>https://openmaps.gov.bc.ca/geo/pub/WHSE_LEGAL_ADMIN_BOUNDARIES.ABMS_REGIONAL_DISTRICTS_SP/ows?service=WMS&amp;request=GetCapabilities</t>
+  </si>
+  <si>
+    <t>https://catalogue.data.gov.bc.ca/dataset/regional-districts-legally-defined-administrative-areas-of-bc</t>
+  </si>
+  <si>
+    <t>WHSE_LEGAL_ADMIN_BOUNDARIES.ABMS_REGIONAL_DISTRICTS_SP</t>
+  </si>
+  <si>
+    <t>ENV Regional Boundaries</t>
+  </si>
+  <si>
+    <t>Environment Regional Boundaries</t>
+  </si>
+  <si>
+    <t>https://openmaps.gov.bc.ca/geo/pub/WHSE_ADMIN_BOUNDARIES.EADM_WLAP_REGION_BND_AREA_SVW/ows?service=WMS&amp;request=GetCapabilities</t>
+  </si>
+  <si>
+    <t>https://catalogue.data.gov.bc.ca/dataset/env-regional-boundaries</t>
+  </si>
+  <si>
+    <t>WHSE_ADMIN_BOUNDARIES.EADM_WLAP_REGION_BND_AREA_SVW</t>
+  </si>
+  <si>
+    <t>BCGW</t>
+  </si>
+  <si>
+    <t>Regions</t>
+  </si>
+  <si>
+    <t>Sections</t>
+  </si>
+  <si>
+    <t>Dataset Name</t>
+  </si>
+  <si>
+    <t>Activities</t>
+  </si>
+  <si>
+    <t>Facilities</t>
+  </si>
+  <si>
+    <t>https://catalogue.data.gov.bc.ca/dataset/bc-wildfire-fire-centres</t>
+  </si>
+  <si>
+    <t>https://catalogue.data.gov.bc.ca/dataset/bc-wildfire-fire-zones</t>
+  </si>
+  <si>
+    <t>FogZone</t>
+  </si>
+  <si>
+    <t>Indicates whether or not the park area overlaps the fog zone, which is along the west coast of Vancouver Island. This is used to indicate campfire ban exceptions.</t>
+  </si>
+  <si>
+    <t>BC Wildfire Fire Centres</t>
+  </si>
+  <si>
+    <t>BC Wildfire Fire Zones; subsections of Fire Centres</t>
+  </si>
+  <si>
+    <t>British Columbia Wildfire Bans and Prohibitions</t>
+  </si>
+  <si>
+    <t>https://catalogue.data.gov.bc.ca/dataset/british-columbia-wildfire-bans-and-prohibitions</t>
+  </si>
+  <si>
+    <t>Wildfire Bans and Prohibitions</t>
+  </si>
+  <si>
+    <t>Reference this to determine campfire ban status for parks.</t>
+  </si>
+  <si>
+    <t>http://bcfireinfo.for.gov.bc.ca/hprScripts/WildfireNews/Bans.asp</t>
+  </si>
+  <si>
+    <t>More Information</t>
+  </si>
+  <si>
+    <t>https://catalogue.data.gov.bc.ca/dataset/bc-wildfire-area-restrictions</t>
+  </si>
+  <si>
+    <t>BC Wildfire Area Restrictions</t>
+  </si>
+  <si>
+    <t>Use on the BC Parks Map to indicate possible affect on park access</t>
+  </si>
+  <si>
+    <t>Wildfire Area Restrictions</t>
+  </si>
+  <si>
+    <t>LicencePlateProjects</t>
+  </si>
+  <si>
+    <t>integrate with ProtectedArea?</t>
+  </si>
+  <si>
+    <t>Campgrounds</t>
+  </si>
+  <si>
+    <t>DayUsePass</t>
+  </si>
+  <si>
+    <t>Indicates whether or not day-use passes are required for this park</t>
+  </si>
+  <si>
+    <t>ParkFireCentreXRef</t>
+  </si>
+  <si>
+    <t>ParkFireZoneXRef</t>
+  </si>
+  <si>
+    <t>not sure if this one is necessary</t>
+  </si>
+  <si>
+    <t>Data Catalogue Record</t>
+  </si>
+  <si>
+    <t>WMS getCapabilities Request URL</t>
+  </si>
+  <si>
+    <t>ParkFogZoneXRef</t>
+  </si>
+  <si>
+    <t>Not sure if this reference method is best</t>
+  </si>
+  <si>
+    <t>Park boundaries can overlap fire zone boundaries; association with multiple fire zones is possible</t>
+  </si>
+  <si>
+    <t>VolunteerPartners</t>
+  </si>
+  <si>
+    <t>ManagementPlanning</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Facility</t>
+  </si>
+  <si>
+    <t>FacilityNumber</t>
+  </si>
+  <si>
+    <t>FacilityName</t>
+  </si>
+  <si>
+    <t>ActivityNumber</t>
+  </si>
+  <si>
+    <t>ActivityName</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>5-10 staff to participate in short testing and development focus and test groups</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Location</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hours</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Maps (park, sites, trails, infrastruture).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Activities/experiences (trails, beach, picnic, etc.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Natural, cultural, or historical features</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Infrastructure (parking, toilets, water, amphitheatre, pump tracks, first aid, electrical, storage, etc.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cell and internet coverage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Accessibility</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pets</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Services (rentals, tours, etc.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calendar of events</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Safety</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Park photos</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Park narrative</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Openings/closures (park)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Openings/closures (trails, beaches etc.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wildlife alerts</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hazards</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Health and safety</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Events</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Facility availability (campsites, parking, etc.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Links to day use permit booking system</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Links to camping booking system</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Links to backcountry permit booking system</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Responsible use messaging</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Jerry’s Rangers materials and activities</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nature, culture, or history</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Links from BC Parks website and Discover Camping</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Social media</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Posters in parks and on materials</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BC Parks will provide information and, where appropriate, introductions relevant to third party partners such as Park Operators, First Nations, NGOs, concessionaires and permit holders.</t>
+    </r>
+  </si>
+  <si>
+    <t>Migrated</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>need to append more data that is not contained in PAR</t>
+  </si>
+  <si>
+    <t>Sites</t>
+  </si>
+  <si>
+    <t>ParkContacts</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>ParkOperatingDates</t>
+  </si>
+  <si>
+    <t>ParkAttendance</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>N?</t>
+  </si>
+  <si>
+    <t>Create a record for this in BCGW</t>
+  </si>
+  <si>
+    <t>Protected Lands</t>
+  </si>
+  <si>
+    <t>Management Areas</t>
+  </si>
+  <si>
+    <t>BC Parks Names</t>
+  </si>
+  <si>
+    <t>Park Details</t>
+  </si>
+  <si>
+    <t>BCGNIS Park Names</t>
+  </si>
+  <si>
+    <t>Park Fees</t>
+  </si>
+  <si>
+    <t>BCPF: Needed from BC Parks</t>
+  </si>
+  <si>
+    <t>ParkActivityXRef</t>
+  </si>
+  <si>
+    <t>ParkFacilityXRef</t>
+  </si>
+  <si>
+    <t>draw the majority of this from AMS API, which is a detailed inventory of individual facilities; we will need to summarize for the park page</t>
+  </si>
+  <si>
+    <t>IconNA</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Path to 'activity available' icon</t>
+  </si>
+  <si>
+    <t>Path to 'activity not available' icon</t>
+  </si>
+  <si>
+    <t>ActivityCode</t>
+  </si>
+  <si>
+    <t>Condensed alpha-only version of the name, currently used to set html element IDs for local page links and element expansion</t>
+  </si>
+  <si>
+    <t>Indicates whether or not the activity type is in use and should be displayed as an option</t>
+  </si>
+  <si>
+    <t>Indicates whether or not the facility type is in use and should be displayed as an option</t>
+  </si>
+  <si>
+    <t>Used to control the sort order of activities</t>
+  </si>
+  <si>
+    <t>FacilityCode</t>
+  </si>
+  <si>
+    <t>Path to 'facility available' icon</t>
+  </si>
+  <si>
+    <t>Path to 'facility not available' icon</t>
+  </si>
+  <si>
+    <t>Used to control the sort order of facilities</t>
+  </si>
+  <si>
+    <t>AssetType</t>
+  </si>
+  <si>
+    <t>AssetTypeNumber</t>
+  </si>
+  <si>
+    <t>AssetCategory</t>
+  </si>
+  <si>
+    <t>Asset Type classification used in the Asset Management System (AMS)</t>
+  </si>
+  <si>
+    <t>Asset Category classification used in the Asset Management System (AMS); parent to Asset Type</t>
+  </si>
+  <si>
+    <t>Link to AssetType</t>
+  </si>
+  <si>
+    <t>Reference to the AMS AssetType</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,12 +1819,49 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
+      <u/>
       <sz val="9"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="12">
@@ -611,7 +1932,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -678,73 +1999,186 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{0B88CCB0-18A3-4823-A563-90BC155E472B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1056,26 +2490,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9256A4-85B0-483D-ABA5-01E16592AE65}">
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:H144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="59.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="76.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="22.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="59.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="4"/>
+    <col min="7" max="7" width="56.83203125" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.33203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1083,7 +2517,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1097,995 +2531,2194 @@
       <c r="G1" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="H1" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-    </row>
-    <row r="4" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
-      <c r="B4" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D5" s="24" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="D7" s="32" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
+      <c r="D8" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="36"/>
       <c r="B9" s="21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="36"/>
-      <c r="B10" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="D9" s="21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
-      <c r="B12" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="C13" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
-      <c r="B14" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="21"/>
+    </row>
+    <row r="15" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
-      <c r="B15" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="21"/>
+    </row>
+    <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="21" t="s">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>97</v>
       </c>
+      <c r="D16" s="21"/>
     </row>
     <row r="17" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
-      <c r="B17" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>97</v>
+      <c r="B17" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
-      <c r="B18" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>97</v>
+      <c r="B18" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
-      <c r="B19" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>94</v>
+      <c r="B19" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
-      <c r="B20" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>65</v>
+      <c r="B20" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="21"/>
+      <c r="G20" s="32" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
-      <c r="B21" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>38</v>
-      </c>
+      <c r="B21" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="32"/>
     </row>
     <row r="22" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
-      <c r="B22" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="C22" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="G22" s="32" t="s">
-        <v>93</v>
-      </c>
+      <c r="B22" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="32"/>
     </row>
     <row r="23" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="36" t="s">
-        <v>116</v>
-      </c>
+      <c r="A23" s="5"/>
       <c r="B23" s="21" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" s="35" t="s">
-        <v>115</v>
+        <v>117</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>35</v>
       </c>
       <c r="G23" s="32"/>
     </row>
     <row r="24" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>57</v>
+      <c r="A24" s="5"/>
+      <c r="B24" s="30" t="s">
+        <v>137</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>115</v>
+        <v>117</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>138</v>
       </c>
       <c r="G24" s="32"/>
     </row>
     <row r="25" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="B25" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="35" t="s">
-        <v>115</v>
+      <c r="A25" s="5"/>
+      <c r="B25" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>152</v>
       </c>
       <c r="G25" s="32"/>
     </row>
     <row r="26" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="D26" s="35" t="s">
-        <v>115</v>
+      <c r="A26" s="5"/>
+      <c r="B26" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>150</v>
       </c>
       <c r="G26" s="32"/>
     </row>
     <row r="27" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
-      <c r="B27" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" s="32" t="s">
-        <v>84</v>
+      <c r="B27" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>154</v>
       </c>
       <c r="G27" s="32"/>
     </row>
     <row r="28" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
-      <c r="B28" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="D28" s="32" t="s">
-        <v>34</v>
+      <c r="B28" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>88</v>
       </c>
       <c r="G28" s="32"/>
     </row>
     <row r="29" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="G29" s="32"/>
     </row>
     <row r="30" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
-      <c r="B30" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E30" s="32" t="s">
-        <v>88</v>
+      <c r="B30" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>25</v>
       </c>
       <c r="G30" s="32"/>
     </row>
     <row r="31" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
-      <c r="B31" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>37</v>
-      </c>
+      <c r="B31" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="21"/>
       <c r="G31" s="32"/>
     </row>
     <row r="32" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
-      <c r="B32" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="B32" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="21"/>
       <c r="G32" s="32"/>
     </row>
     <row r="33" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
-      <c r="B33" s="25" t="s">
-        <v>45</v>
+      <c r="B33" s="30" t="s">
+        <v>47</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>99</v>
+        <v>95</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>114</v>
       </c>
       <c r="G33" s="32"/>
     </row>
     <row r="34" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
-      <c r="B34" s="25" t="s">
-        <v>46</v>
+      <c r="B34" s="21" t="s">
+        <v>10</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="G34" s="32"/>
+        <v>96</v>
+      </c>
+      <c r="D34" s="21"/>
     </row>
     <row r="35" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
-      <c r="B35" s="25" t="s">
-        <v>47</v>
+      <c r="B35" s="21" t="s">
+        <v>11</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="D35" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="G35" s="32"/>
+        <v>97</v>
+      </c>
+      <c r="D35" s="21"/>
     </row>
     <row r="36" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5"/>
       <c r="B36" s="21" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C36" s="21" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
+      <c r="D36" s="21"/>
+    </row>
+    <row r="37" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="9"/>
       <c r="B37" s="21" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C37" s="21" t="s">
         <v>97</v>
       </c>
+      <c r="D37" s="21"/>
     </row>
     <row r="38" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
-      <c r="B38" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
-      <c r="B39" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="21" t="s">
+    </row>
+    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="40" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="14"/>
+      <c r="B42" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="14"/>
+      <c r="B43" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="16"/>
+      <c r="B44" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A46" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="33" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="20"/>
+      <c r="B47" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="10" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="5"/>
-    </row>
-    <row r="41" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="41" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="14"/>
-      <c r="B44" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="14"/>
-      <c r="B45" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="16"/>
-      <c r="B46" s="17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A48" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="33" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="20"/>
-      <c r="B49" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C49" s="10" t="s">
+      <c r="D47" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="E47" s="32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="37"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="5"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="45"/>
+      <c r="E50" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="G50" s="44" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="5"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="G51" s="19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="5"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="G52" s="19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="5"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G53" s="19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="5"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="G54" s="19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+    </row>
+    <row r="57" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="5"/>
+      <c r="B57" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="D49" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="E49" s="32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="37"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="E51" s="32"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="5"/>
-      <c r="B52" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C52" s="21" t="s">
+      <c r="D57" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="5"/>
+    </row>
+    <row r="59" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B59" s="27"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="5"/>
+      <c r="B60" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C60" s="21" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B54" s="27"/>
-      <c r="C54" s="27"/>
-    </row>
-    <row r="55" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="5"/>
-      <c r="B55" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C55" s="21" t="s">
+    <row r="61" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="5"/>
+    </row>
+    <row r="62" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B62" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="D55" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="5"/>
-    </row>
-    <row r="57" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="B57" s="27"/>
-      <c r="C57" s="27"/>
-      <c r="D57" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="5"/>
-      <c r="B58" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C58" s="21" t="s">
+      <c r="D62" s="26"/>
+      <c r="E62" s="27"/>
+      <c r="F62" s="27"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="20"/>
+      <c r="B63" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C63" s="10" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="5"/>
-    </row>
-    <row r="60" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="B60" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C60" s="27" t="s">
+      <c r="D63" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="20"/>
+      <c r="B64" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C64" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D60" s="26"/>
-      <c r="E60" s="27"/>
-      <c r="F60" s="27"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="20"/>
-      <c r="B61" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="20"/>
-      <c r="B62" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C62" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="7"/>
-      <c r="B63" s="8"/>
-      <c r="C63" s="6"/>
-    </row>
-    <row r="64" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="26" t="s">
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="7"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="6"/>
+    </row>
+    <row r="66" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B64" s="27"/>
-      <c r="C64" s="27"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="18"/>
-      <c r="F64" s="4" t="s">
+      <c r="B66" s="27"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="4" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="5"/>
-      <c r="B65" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C65" s="22"/>
-    </row>
-    <row r="66" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="5"/>
-      <c r="B66" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C66" s="21"/>
-      <c r="D66" s="6" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="5"/>
-      <c r="B67" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C67" s="21"/>
+      <c r="B67" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" s="22"/>
     </row>
     <row r="68" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="5"/>
       <c r="B68" s="21" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C68" s="21"/>
+      <c r="D68" s="6" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="69" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="5"/>
-      <c r="B69" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="C69" s="28"/>
-      <c r="G69" s="19" t="s">
-        <v>133</v>
-      </c>
+      <c r="B69" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C69" s="21"/>
     </row>
     <row r="70" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="5"/>
       <c r="B70" s="21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C70" s="21"/>
     </row>
     <row r="71" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="5"/>
-      <c r="B71" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C71" s="21"/>
-      <c r="D71" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="B71" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="C71" s="28"/>
+      <c r="G71" s="32"/>
     </row>
     <row r="72" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="5"/>
       <c r="B72" s="21" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C72" s="21"/>
     </row>
     <row r="73" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="5"/>
       <c r="B73" s="21" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C73" s="21"/>
+      <c r="D73" s="6" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="74" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="5"/>
-      <c r="B74" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C74" s="21"/>
+      <c r="B74" s="52" t="s">
+        <v>241</v>
+      </c>
+      <c r="C74" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="D74" s="53" t="s">
+        <v>242</v>
+      </c>
+      <c r="G74" s="53" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="75" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="5"/>
       <c r="B75" s="21" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C75" s="21"/>
     </row>
     <row r="76" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="5"/>
       <c r="B76" s="21" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C76" s="21"/>
     </row>
     <row r="77" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="5"/>
       <c r="B77" s="21" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="C77" s="21"/>
     </row>
     <row r="78" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="5"/>
       <c r="B78" s="21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C78" s="21"/>
     </row>
     <row r="79" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="5"/>
       <c r="B79" s="21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C79" s="21"/>
     </row>
     <row r="80" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="5"/>
       <c r="B80" s="21" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="C80" s="21"/>
     </row>
     <row r="81" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="5"/>
       <c r="B81" s="21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C81" s="21"/>
-      <c r="D81" s="35" t="s">
-        <v>114</v>
-      </c>
     </row>
     <row r="82" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="5"/>
       <c r="B82" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C82" s="21"/>
+    </row>
+    <row r="83" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="5"/>
+      <c r="B83" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C83" s="21"/>
+    </row>
+    <row r="84" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="5"/>
+      <c r="B84" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C84" s="21"/>
+      <c r="D84" s="32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="5"/>
+      <c r="B85" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C82" s="31" t="s">
+      <c r="C85" s="31" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="83" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="9"/>
-      <c r="B83" s="30" t="s">
+    <row r="86" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="5"/>
+      <c r="B86" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="C86" s="21"/>
+      <c r="D86" s="51" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="5"/>
+      <c r="B87" s="52" t="s">
+        <v>258</v>
+      </c>
+      <c r="C87" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="D87" s="53" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="9"/>
+      <c r="B88" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C83" s="31" t="s">
+      <c r="C88" s="31" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="26" t="s">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B85" s="27"/>
-      <c r="C85" s="27"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B86" s="42" t="s">
+      <c r="B90" s="27"/>
+      <c r="C90" s="27"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B91" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C91" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="D91" s="43"/>
+      <c r="E91" s="43"/>
+      <c r="F91" s="43"/>
+      <c r="G91" s="43" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" s="4"/>
+      <c r="B92" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="C86" s="22"/>
-      <c r="G86" s="45" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="4"/>
-      <c r="B87" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="C87" s="21"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B88" s="24" t="s">
+      <c r="C92" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D92" s="43"/>
+      <c r="E92" s="43"/>
+      <c r="F92" s="43"/>
+      <c r="G92" s="43"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B93" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="C93" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D93" s="43"/>
+      <c r="E93" s="43"/>
+      <c r="F93" s="43"/>
+      <c r="G93" s="43"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B94" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C94" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D94" s="43"/>
+      <c r="E94" s="43"/>
+      <c r="F94" s="43"/>
+      <c r="G94" s="43"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B95" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C95" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D95" s="43"/>
+      <c r="E95" s="43"/>
+      <c r="F95" s="43"/>
+      <c r="G95" s="43" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B96" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C96" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D96" s="43"/>
+      <c r="E96" s="43"/>
+      <c r="F96" s="43"/>
+      <c r="G96" s="43" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B97" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C97" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B98" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C98" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B99" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C99" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B100" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C100" s="21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B101" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="C88" s="21"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B89" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C89" s="21"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B90" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C90" s="21"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B91" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C91" s="21"/>
-      <c r="G91" s="45" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B92" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C92" s="21"/>
-      <c r="G92" s="45" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B93" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C93" s="21"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B94" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C94" s="21"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B95" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C95" s="21"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B96" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C96" s="21"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B97" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C97" s="19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B98" s="19" t="s">
+      <c r="C101" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="D101" s="44" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B102" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C98" s="19" t="s">
+      <c r="C102" s="30" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B100" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="C100" s="27"/>
-      <c r="F100" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G100" s="46" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B101" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="C101" s="22"/>
-      <c r="G101" s="46"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B102" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C102" s="21"/>
-      <c r="D102" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G102" s="46"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G103" s="46"/>
+      <c r="D102" s="44" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B104" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="C104" s="27"/>
+        <v>112</v>
+      </c>
+      <c r="C104" s="27" t="s">
+        <v>95</v>
+      </c>
       <c r="F104" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G104" s="46"/>
+      <c r="G104" s="60" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B105" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="C105" s="22"/>
-      <c r="G105" s="46"/>
+        <v>121</v>
+      </c>
+      <c r="C105" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="G105" s="60"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B106" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C106" s="21"/>
       <c r="D106" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G106" s="46"/>
+        <v>72</v>
+      </c>
+      <c r="G106" s="60"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F107" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G107" s="46"/>
+      <c r="G107" s="60"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B108" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="C108" s="27"/>
+        <v>111</v>
+      </c>
+      <c r="C108" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G108" s="60"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B109" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="C109" s="22"/>
+        <v>122</v>
+      </c>
+      <c r="C109" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="G109" s="60"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B110" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C110" s="21"/>
+      <c r="D110" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G110" s="60"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F111" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G111" s="60"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B112" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C112" s="27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B113" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C113" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="B115" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="C115" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D115" s="48" t="s">
+        <v>243</v>
+      </c>
+      <c r="F115" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="H115" s="55" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B116" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="C116" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B117" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C117" s="21"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="B119" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="C119" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D119" s="48" t="s">
+        <v>244</v>
+      </c>
+      <c r="F119" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="H119" s="58" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B120" s="42" t="s">
+        <v>163</v>
+      </c>
+      <c r="C120" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B121" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="C121" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A123" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="B123" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="C123" s="27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B124" s="42" t="s">
+        <v>275</v>
+      </c>
+      <c r="C124" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B125" s="42" t="s">
+        <v>334</v>
+      </c>
+      <c r="C125" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B126" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="C126" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B127" s="21" t="s">
+        <v>330</v>
+      </c>
+      <c r="C127" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D127" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B128" s="21" t="s">
+        <v>331</v>
+      </c>
+      <c r="C128" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D128" s="48" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B129" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C129" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B130" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C130" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="B132" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="C132" s="27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B133" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="C133" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B134" s="42" t="s">
+        <v>339</v>
+      </c>
+      <c r="C134" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D134" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B135" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="C135" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B136" s="21" t="s">
+        <v>330</v>
+      </c>
+      <c r="C136" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B137" s="21" t="s">
+        <v>331</v>
+      </c>
+      <c r="C137" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D137" s="48" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B138" s="21" t="s">
+        <v>343</v>
+      </c>
+      <c r="C138" s="31" t="s">
+        <v>348</v>
+      </c>
+      <c r="D138" s="48" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B139" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C139" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D139" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B140" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C140" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="D140" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" s="26" t="s">
+        <v>343</v>
+      </c>
+      <c r="B142" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="C142" s="27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B143" s="56" t="s">
+        <v>343</v>
+      </c>
+      <c r="C143" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="D143" s="4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B144" s="56" t="s">
+        <v>345</v>
+      </c>
+      <c r="C144" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="D144" s="4" t="s">
+        <v>347</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G100:G107"/>
+    <mergeCell ref="G104:G111"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H115" r:id="rId1" xr:uid="{C542003A-DE46-4D98-A11B-9CC195E7F11A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="90" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="90" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171C08A0-AF00-4BB5-82D1-824633A7E054}">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="51" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="41.1640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="62.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="64" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.33203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="46" t="s">
+        <v>263</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>264</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="46" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>180</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>185</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>189</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>192</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="56" t="s">
+        <v>245</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>246</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="56" t="s">
+        <v>248</v>
+      </c>
+      <c r="G8" s="57" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="56" t="s">
+        <v>252</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>251</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>254</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="50" t="s">
+        <v>253</v>
+      </c>
+      <c r="G9" s="21"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>196</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="D10" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="G11" s="21"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>204</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>208</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>213</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="D14" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>217</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="B16" s="47" t="s">
+        <v>221</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="D16" s="47" t="s">
+        <v>220</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>225</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>231</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D17" r:id="rId1" xr:uid="{F1535CA5-FED5-4987-AFF5-0D4FF1813E5A}"/>
+    <hyperlink ref="D7" r:id="rId2" xr:uid="{6B885E05-3FFA-403D-870B-0F1880316E45}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{8522FD56-F6F3-472F-B428-D9116BB0B073}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{FDE51DB0-BE3E-47D9-A26D-D6DE9B4912F6}"/>
+    <hyperlink ref="D2" r:id="rId5" xr:uid="{1F930894-9A84-4455-902B-339A973EA021}"/>
+    <hyperlink ref="D14" r:id="rId6" xr:uid="{91FA6640-3495-42D2-86ED-A382BB0B8B07}"/>
+    <hyperlink ref="D4" r:id="rId7" xr:uid="{68641987-56C1-4CD4-B754-BA867FDFC02C}"/>
+    <hyperlink ref="D5" r:id="rId8" xr:uid="{2C0BDE24-1C77-420D-A50A-51EC3A357F0E}"/>
+    <hyperlink ref="D18" r:id="rId9" xr:uid="{724F0ACC-D6E6-4F14-A902-16823B214B6C}"/>
+    <hyperlink ref="D12" r:id="rId10" xr:uid="{D3F18D35-E48A-4BE8-9517-BC7B4C156D33}"/>
+    <hyperlink ref="D13" r:id="rId11" xr:uid="{8AD3BD51-9926-4A6C-AB86-778193A171D6}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{B7FADF48-BE59-4185-936C-170A112108BC}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{68C92683-9104-4846-ACB0-2C30A0DC646F}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{0AD74F1C-479E-4610-A952-DB583AD06D1D}"/>
+    <hyperlink ref="B6" r:id="rId15" xr:uid="{04AE96E0-2A71-47E3-B9CF-3B781421C5A5}"/>
+    <hyperlink ref="B4" r:id="rId16" xr:uid="{6FC94149-11CD-4460-9899-7737271E0CAB}"/>
+    <hyperlink ref="B5" r:id="rId17" xr:uid="{D6C22A79-A0D7-46B0-96EB-2CCAFED3254D}"/>
+    <hyperlink ref="B12" r:id="rId18" xr:uid="{92981390-F9DB-4B3E-8F49-BA28333788D8}"/>
+    <hyperlink ref="B15" r:id="rId19" xr:uid="{25FE8EDF-4861-497E-9DAA-D4353A237380}"/>
+    <hyperlink ref="B16" r:id="rId20" xr:uid="{EFA23A56-88FD-4540-AA12-6F1CFAD9723F}"/>
+    <hyperlink ref="D16" r:id="rId21" xr:uid="{F8B55FCA-7F82-477E-AF79-7B19336DFE86}"/>
+    <hyperlink ref="B2" r:id="rId22" xr:uid="{6FE19610-58B4-48D8-BED7-41FBCB76D58F}"/>
+    <hyperlink ref="B3" r:id="rId23" xr:uid="{41DE1A15-E9AE-4DFC-842B-2D753AA2C4ED}"/>
+    <hyperlink ref="B17" r:id="rId24" xr:uid="{AA36631E-4E53-43DC-9855-E27FC2CC07DD}"/>
+    <hyperlink ref="B18" r:id="rId25" xr:uid="{B782DF9B-659E-4BD0-824B-0DB4125E2DB6}"/>
+    <hyperlink ref="B10" r:id="rId26" xr:uid="{11339830-CD8A-4BE4-B8AB-6AB85EC22571}"/>
+    <hyperlink ref="D10" r:id="rId27" xr:uid="{C865944A-F024-471E-B258-ECBE758EFDB2}"/>
+    <hyperlink ref="B11" r:id="rId28" xr:uid="{C4AD4FC0-B258-4BDE-B189-DCDF80E94F1E}"/>
+    <hyperlink ref="D11" r:id="rId29" xr:uid="{1C6CF777-5B13-4BD3-A2BB-D27CC6AB09DE}"/>
+    <hyperlink ref="B8" r:id="rId30" xr:uid="{1CB2EC76-E679-47F0-B6BA-E7E34718D1BC}"/>
+    <hyperlink ref="G8" r:id="rId31" xr:uid="{1451B9F1-A0CE-4796-A76F-4E624E0228FE}"/>
+    <hyperlink ref="B9" r:id="rId32" xr:uid="{93F08A46-02D3-402D-8664-C986F130162E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId33"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8188FD92-A7C9-4AC5-9D59-53B6660F6045}">
+  <dimension ref="A1:I33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.1640625" style="72" customWidth="1"/>
+    <col min="2" max="3" width="9" style="59" customWidth="1"/>
+    <col min="4" max="4" width="52.83203125" style="72" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="9.33203125" style="4"/>
+    <col min="9" max="9" width="137.33203125" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="9.33203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="65" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>309</v>
+      </c>
+      <c r="C1" s="65" t="s">
+        <v>310</v>
+      </c>
+      <c r="D1" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="61" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="66" t="s">
+        <v>320</v>
+      </c>
+      <c r="B2" s="67" t="s">
+        <v>314</v>
+      </c>
+      <c r="C2" s="67" t="s">
+        <v>314</v>
+      </c>
+      <c r="D2" s="68" t="s">
+        <v>311</v>
+      </c>
+      <c r="I2" s="62" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="66" t="s">
+        <v>312</v>
+      </c>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="68" t="s">
+        <v>311</v>
+      </c>
+      <c r="I3" s="63" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="66" t="s">
+        <v>234</v>
+      </c>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="68"/>
+      <c r="I4" s="63" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="66" t="s">
+        <v>235</v>
+      </c>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="68"/>
+      <c r="I5" s="63" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="66" t="s">
+        <v>321</v>
+      </c>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="68"/>
+      <c r="I6" s="63" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="69" t="s">
+        <v>237</v>
+      </c>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="68"/>
+      <c r="I7" s="63" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="73" t="s">
+        <v>327</v>
+      </c>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="68"/>
+      <c r="I8" s="63" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="36" x14ac:dyDescent="0.2">
+      <c r="A9" s="69" t="s">
+        <v>238</v>
+      </c>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="68" t="s">
+        <v>329</v>
+      </c>
+      <c r="I9" s="63" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="73" t="s">
+        <v>328</v>
+      </c>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="68"/>
+      <c r="I10" s="63" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="69" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="68"/>
+      <c r="I11" s="63" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="69" t="s">
+        <v>191</v>
+      </c>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="68"/>
+      <c r="I12" s="63" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="73" t="s">
+        <v>260</v>
+      </c>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="71" t="s">
+        <v>262</v>
+      </c>
+      <c r="I13" s="63" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="73" t="s">
+        <v>261</v>
+      </c>
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="68"/>
+      <c r="I14" s="63" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="73" t="s">
+        <v>265</v>
+      </c>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="68"/>
+      <c r="I15" s="63" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="69" t="s">
+        <v>322</v>
+      </c>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="71" t="s">
+        <v>256</v>
+      </c>
+      <c r="I16" s="64" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="69" t="s">
+        <v>324</v>
+      </c>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="71"/>
+      <c r="I17" s="63" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="69" t="s">
+        <v>323</v>
+      </c>
+      <c r="B18" s="70"/>
+      <c r="C18" s="67" t="s">
+        <v>317</v>
+      </c>
+      <c r="D18" s="68"/>
+      <c r="I18" s="63" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="69" t="s">
+        <v>325</v>
+      </c>
+      <c r="B19" s="70"/>
+      <c r="C19" s="67" t="s">
+        <v>317</v>
+      </c>
+      <c r="D19" s="68"/>
+      <c r="I19" s="63" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="69" t="s">
+        <v>257</v>
+      </c>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="68" t="s">
+        <v>319</v>
+      </c>
+      <c r="I20" s="63" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="69" t="s">
+        <v>255</v>
+      </c>
+      <c r="B21" s="70"/>
+      <c r="C21" s="67" t="s">
+        <v>317</v>
+      </c>
+      <c r="D21" s="68"/>
+      <c r="I21" s="63" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="69" t="s">
+        <v>268</v>
+      </c>
+      <c r="B22" s="70"/>
+      <c r="C22" s="67" t="s">
+        <v>318</v>
+      </c>
+      <c r="D22" s="68"/>
+      <c r="I22" s="63" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="69" t="s">
+        <v>269</v>
+      </c>
+      <c r="B23" s="70"/>
+      <c r="C23" s="67" t="s">
+        <v>317</v>
+      </c>
+      <c r="D23" s="68"/>
+      <c r="I23" s="64" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="69" t="s">
+        <v>313</v>
+      </c>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="68"/>
+      <c r="I24" s="63" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="69" t="s">
+        <v>315</v>
+      </c>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67" t="s">
+        <v>317</v>
+      </c>
+      <c r="D25" s="68"/>
+      <c r="I25" s="63" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="69" t="s">
+        <v>316</v>
+      </c>
+      <c r="B26" s="67"/>
+      <c r="C26" s="67" t="s">
+        <v>314</v>
+      </c>
+      <c r="D26" s="68"/>
+      <c r="I26" s="64" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I27" s="63" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I28" s="63" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="64" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I30" s="63" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I31" s="63" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="64" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I33" s="64" t="s">
+        <v>308</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D7ED20A-5A3A-453C-8A81-923C8953B4C9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66662F61-F679-43AD-99EF-C80D953E466D}">
   <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="59.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="76.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="22.1640625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="19.83203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="59.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="4"/>
+    <col min="7" max="7" width="76.5" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.33203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2915,7 +5548,7 @@
       <c r="F95" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G95" s="46" t="s">
+      <c r="G95" s="60" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2924,7 +5557,7 @@
         <v>66</v>
       </c>
       <c r="C96" s="22"/>
-      <c r="G96" s="46"/>
+      <c r="G96" s="60"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B97" s="21" t="s">
@@ -2934,10 +5567,10 @@
       <c r="D97" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G97" s="46"/>
+      <c r="G97" s="60"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G98" s="46"/>
+      <c r="G98" s="60"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="26" t="s">
@@ -2950,14 +5583,14 @@
       <c r="F99" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G99" s="46"/>
+      <c r="G99" s="60"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B100" s="22" t="s">
         <v>66</v>
       </c>
       <c r="C100" s="22"/>
-      <c r="G100" s="46"/>
+      <c r="G100" s="60"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B101" s="21" t="s">
@@ -2967,13 +5600,13 @@
       <c r="D101" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G101" s="46"/>
+      <c r="G101" s="60"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F102" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G102" s="46"/>
+      <c r="G102" s="60"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="26" t="s">
@@ -2996,16 +5629,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D7ED20A-5A3A-453C-8A81-923C8953B4C9}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
NOBUG: Updating model and dataset docs
</commit_message>
<xml_diff>
--- a/docs/BC Parks CMS Data Model.xlsx
+++ b/docs/BC Parks CMS Data Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rofiddle\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF999796-8CFD-4F11-925D-6DA14C516D60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5F4106-D3EE-4866-83D5-9C5D13FDE2E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A33082D8-1C98-4870-8924-9924FABEACC5}"/>
+    <workbookView xWindow="-21825" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{A33082D8-1C98-4870-8924-9924FABEACC5}"/>
   </bookViews>
   <sheets>
     <sheet name="BCParks" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="475">
   <si>
     <t>Table</t>
   </si>
@@ -1694,12 +1694,21 @@
   <si>
     <t>Indicates the date/time that the off-season ends</t>
   </si>
+  <si>
+    <t>ParkFees</t>
+  </si>
+  <si>
+    <t>Relates to a park activity or facility</t>
+  </si>
+  <si>
+    <t>Link to ParkFeatures</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1"/>
@@ -1875,11 +1884,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="11">
@@ -2085,7 +2089,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2186,8 +2190,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2200,7 +2204,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" customBuiltin="1"/>
@@ -2522,11 +2525,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9256A4-85B0-483D-ABA5-01E16592AE65}">
-  <dimension ref="A1:J346"/>
+  <dimension ref="A1:J353"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C264" sqref="C264"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2812,7 +2815,7 @@
     </row>
     <row r="15" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="38" t="s">
         <v>169</v>
       </c>
       <c r="C15" s="38" t="s">
@@ -2821,7 +2824,7 @@
       <c r="D15" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="44" t="b">
+      <c r="E15" s="21" t="b">
         <v>0</v>
       </c>
       <c r="F15" s="21" t="s">
@@ -2830,7 +2833,7 @@
     </row>
     <row r="16" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="38" t="s">
         <v>361</v>
       </c>
       <c r="C16" s="27" t="s">
@@ -3969,7 +3972,7 @@
       <c r="I101" s="18"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A102" s="67"/>
+      <c r="A102" s="66"/>
       <c r="B102" s="29" t="s">
         <v>399</v>
       </c>
@@ -3982,95 +3985,88 @@
         <v>401</v>
       </c>
     </row>
-    <row r="103" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="4"/>
-      <c r="B103" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="C103" s="18"/>
-      <c r="D103" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E103" s="18"/>
-      <c r="F103" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="G103" s="18"/>
-      <c r="H103" s="18"/>
-      <c r="I103" s="18"/>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" s="66"/>
+      <c r="B103" s="29" t="s">
+        <v>441</v>
+      </c>
+      <c r="C103" s="21"/>
+      <c r="D103" s="20" t="s">
+        <v>474</v>
+      </c>
+      <c r="E103" s="23"/>
+      <c r="F103" s="36"/>
     </row>
     <row r="104" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4"/>
       <c r="B104" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="C104" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="D104" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="C104" s="18"/>
+      <c r="D104" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E104" s="20"/>
+      <c r="E104" s="18"/>
       <c r="F104" s="21" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="G104" s="18"/>
       <c r="H104" s="18"/>
       <c r="I104" s="18"/>
     </row>
-    <row r="105" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="6"/>
+    <row r="105" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="4"/>
       <c r="B105" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="C105" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="C105" s="18" t="s">
+        <v>272</v>
+      </c>
       <c r="D105" s="20" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E105" s="20"/>
-      <c r="F105" s="18"/>
+      <c r="F105" s="21" t="s">
+        <v>90</v>
+      </c>
       <c r="G105" s="18"/>
       <c r="H105" s="18"/>
       <c r="I105" s="18"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C106" s="23"/>
-      <c r="D106" s="36"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A108" s="11" t="s">
+    <row r="106" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="6"/>
+      <c r="B106" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="C106" s="18"/>
+      <c r="D106" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E106" s="20"/>
+      <c r="F106" s="18"/>
+      <c r="G106" s="18"/>
+      <c r="H106" s="18"/>
+      <c r="I106" s="18"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C107" s="23"/>
+      <c r="D107" s="36"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A109" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B108" s="25"/>
-      <c r="C108" s="25"/>
-      <c r="D108" s="25"/>
-      <c r="E108" s="35"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B109" s="21" t="s">
+      <c r="B109" s="25"/>
+      <c r="C109" s="25"/>
+      <c r="D109" s="25"/>
+      <c r="E109" s="35"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B110" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="C109" s="21" t="s">
+      <c r="C110" s="21" t="s">
         <v>203</v>
-      </c>
-      <c r="D109" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E109" s="23"/>
-      <c r="F109" s="36"/>
-      <c r="G109" s="36"/>
-      <c r="H109" s="36"/>
-      <c r="I109" s="36" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A110" s="17"/>
-      <c r="B110" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="C110" s="21" t="s">
-        <v>204</v>
       </c>
       <c r="D110" s="21" t="s">
         <v>47</v>
@@ -4079,17 +4075,20 @@
       <c r="F110" s="36"/>
       <c r="G110" s="36"/>
       <c r="H110" s="36"/>
-      <c r="I110" s="36"/>
+      <c r="I110" s="36" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" s="17"/>
       <c r="B111" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C111" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D111" s="21" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E111" s="23"/>
       <c r="F111" s="36"/>
@@ -4099,13 +4098,13 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B112" s="21" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C112" s="21" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="D112" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E112" s="23"/>
       <c r="F112" s="36"/>
@@ -4115,28 +4114,26 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B113" s="21" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C113" s="21" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D113" s="21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E113" s="23"/>
       <c r="F113" s="36"/>
       <c r="G113" s="36"/>
       <c r="H113" s="36"/>
-      <c r="I113" s="36" t="s">
-        <v>62</v>
-      </c>
+      <c r="I113" s="36"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B114" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C114" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D114" s="21" t="s">
         <v>46</v>
@@ -4151,34 +4148,40 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B115" s="21" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="C115" s="21" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="D115" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E115" s="19"/>
+        <v>46</v>
+      </c>
+      <c r="E115" s="23"/>
+      <c r="F115" s="36"/>
+      <c r="G115" s="36"/>
+      <c r="H115" s="36"/>
+      <c r="I115" s="36" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B116" s="21" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="C116" s="21" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="D116" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E116" s="19"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B117" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C117" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D117" s="21" t="s">
         <v>48</v>
@@ -4187,818 +4190,816 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B118" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C118" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D118" s="21" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E118" s="19"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B119" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="C119" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="D119" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E119" s="19"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B120" s="21" t="s">
         <v>349</v>
       </c>
-      <c r="C119" s="21"/>
-      <c r="D119" s="21" t="s">
+      <c r="C120" s="21"/>
+      <c r="D120" s="21" t="s">
         <v>60</v>
-      </c>
-      <c r="E119" s="23"/>
-      <c r="F119" s="36" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A120" s="67"/>
-      <c r="B120" s="29" t="s">
-        <v>399</v>
-      </c>
-      <c r="C120" s="21"/>
-      <c r="D120" s="20" t="s">
-        <v>400</v>
       </c>
       <c r="E120" s="23"/>
       <c r="F120" s="36" t="s">
-        <v>401</v>
+        <v>79</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B121" s="21" t="s">
-        <v>177</v>
+      <c r="A121" s="66"/>
+      <c r="B121" s="29" t="s">
+        <v>399</v>
       </c>
       <c r="C121" s="21"/>
-      <c r="D121" s="21" t="s">
-        <v>47</v>
+      <c r="D121" s="20" t="s">
+        <v>400</v>
       </c>
       <c r="E121" s="23"/>
       <c r="F121" s="36" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A122" s="66"/>
+      <c r="B122" s="29" t="s">
+        <v>441</v>
+      </c>
+      <c r="C122" s="21"/>
+      <c r="D122" s="20" t="s">
+        <v>474</v>
+      </c>
+      <c r="E122" s="23"/>
+      <c r="F122" s="36"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B123" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C123" s="21"/>
+      <c r="D123" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E123" s="23"/>
+      <c r="F123" s="36" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B122" s="21"/>
-      <c r="C122" s="21" t="s">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B124" s="21"/>
+      <c r="C124" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="D122" s="21" t="s">
+      <c r="D124" s="21" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C123" s="45"/>
-      <c r="D123" s="56"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A124" s="11" t="s">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C125" s="45"/>
+      <c r="D125" s="56"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A126" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B124" s="25"/>
-      <c r="C124" s="25"/>
-      <c r="D124" s="25"/>
-      <c r="E124" s="35"/>
-      <c r="H124" s="17" t="s">
+      <c r="B126" s="25"/>
+      <c r="C126" s="25"/>
+      <c r="D126" s="25"/>
+      <c r="E126" s="35"/>
+      <c r="H126" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="I124" s="68" t="s">
+      <c r="I126" s="68" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A125" s="55"/>
-      <c r="B125" s="21" t="s">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A127" s="55"/>
+      <c r="B127" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="C125" s="21" t="s">
+      <c r="C127" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="D125" s="21" t="s">
+      <c r="D127" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E125" s="35"/>
-      <c r="I125" s="68"/>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B126" s="21" t="s">
+      <c r="E127" s="35"/>
+      <c r="I127" s="68"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B128" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="C126" s="21" t="s">
+      <c r="C128" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="D126" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E126" s="19"/>
-      <c r="I126" s="68"/>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B127" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C127" s="21" t="s">
-        <v>327</v>
-      </c>
-      <c r="D127" s="21"/>
-      <c r="E127" s="19"/>
-      <c r="F127" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I127" s="68"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B128" s="21"/>
-      <c r="C128" s="21" t="s">
-        <v>320</v>
-      </c>
       <c r="D128" s="21" t="s">
-        <v>338</v>
+        <v>47</v>
       </c>
       <c r="E128" s="19"/>
       <c r="I128" s="68"/>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B129" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C129" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="D129" s="21"/>
+      <c r="E129" s="19"/>
+      <c r="F129" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="I129" s="68"/>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A130" s="11" t="s">
+      <c r="B130" s="21"/>
+      <c r="C130" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="D130" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="E130" s="19"/>
+      <c r="I130" s="68"/>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I131" s="68"/>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A132" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B130" s="25"/>
-      <c r="C130" s="25"/>
-      <c r="D130" s="25" t="s">
+      <c r="B132" s="25"/>
+      <c r="C132" s="25"/>
+      <c r="D132" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E130" s="35"/>
-      <c r="H130" s="17" t="s">
+      <c r="E132" s="35"/>
+      <c r="H132" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="I130" s="68"/>
-    </row>
-    <row r="131" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="B131" s="21" t="s">
+      <c r="I132" s="68"/>
+    </row>
+    <row r="133" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="B133" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="C131" s="21" t="s">
+      <c r="C133" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="D131" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E131" s="19"/>
-      <c r="I131" s="68"/>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B132" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="C132" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D132" s="21"/>
-      <c r="E132" s="19"/>
-      <c r="F132" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="I132" s="68"/>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B133" s="21"/>
-      <c r="C133" s="21" t="s">
-        <v>311</v>
-      </c>
-      <c r="D133" s="21"/>
+      <c r="D133" s="21" t="s">
+        <v>47</v>
+      </c>
       <c r="E133" s="19"/>
       <c r="I133" s="68"/>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B134" s="21" t="s">
-        <v>25</v>
+        <v>209</v>
       </c>
       <c r="C134" s="21" t="s">
-        <v>320</v>
+        <v>209</v>
       </c>
       <c r="D134" s="21"/>
       <c r="E134" s="19"/>
+      <c r="F134" s="17" t="s">
+        <v>30</v>
+      </c>
       <c r="I134" s="68"/>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B135" s="54"/>
-      <c r="C135" s="54"/>
-      <c r="D135" s="54"/>
+      <c r="B135" s="21"/>
+      <c r="C135" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="D135" s="21"/>
       <c r="E135" s="19"/>
       <c r="I135" s="68"/>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H136" s="17" t="s">
+      <c r="B136" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C136" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="D136" s="21"/>
+      <c r="E136" s="19"/>
+      <c r="I136" s="68"/>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B137" s="54"/>
+      <c r="C137" s="54"/>
+      <c r="D137" s="54"/>
+      <c r="E137" s="19"/>
+      <c r="I137" s="68"/>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H138" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="I136" s="68"/>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A137" s="11" t="s">
+      <c r="I138" s="68"/>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A139" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B137" s="25" t="s">
+      <c r="B139" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="C137" s="25"/>
-      <c r="D137" s="25" t="s">
+      <c r="C139" s="25"/>
+      <c r="D139" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E137" s="35"/>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B138" s="38" t="s">
+      <c r="E139" s="35"/>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B140" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="C138" s="38"/>
-      <c r="D138" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E138" s="19"/>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A140" s="11" t="s">
+      <c r="C140" s="38"/>
+      <c r="D140" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E140" s="19"/>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A142" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B140" s="11"/>
-      <c r="C140" s="11"/>
-      <c r="D140" s="11"/>
-      <c r="E140" s="35"/>
-      <c r="F140" s="17" t="s">
+      <c r="B142" s="11"/>
+      <c r="C142" s="11"/>
+      <c r="D142" s="11"/>
+      <c r="E142" s="35"/>
+      <c r="F142" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="H140" s="17" t="s">
+      <c r="H142" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="J140" s="39" t="s">
+      <c r="J142" s="39" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B141" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="C141" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="D141" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E141" s="19"/>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B142" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="C142" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="D142" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E142" s="19"/>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B143" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="C143" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="D143" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E143" s="19"/>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B144" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="C144" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="D144" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E144" s="19"/>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B145" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="C143" s="21" t="s">
+      <c r="C145" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="D143" s="21"/>
-      <c r="E143" s="19"/>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A145" s="11" t="s">
+      <c r="D145" s="21"/>
+      <c r="E145" s="19"/>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A147" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B145" s="11"/>
-      <c r="C145" s="11"/>
-      <c r="D145" s="11"/>
-      <c r="E145" s="35"/>
-      <c r="F145" s="17" t="s">
+      <c r="B147" s="11"/>
+      <c r="C147" s="11"/>
+      <c r="D147" s="11"/>
+      <c r="E147" s="35"/>
+      <c r="F147" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="H145" s="17" t="s">
+      <c r="H147" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="I145" s="23" t="s">
+      <c r="I147" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="J145" s="22" t="s">
+      <c r="J147" s="22" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B146" s="21" t="s">
-        <v>214</v>
-      </c>
-      <c r="C146" s="21" t="s">
-        <v>214</v>
-      </c>
-      <c r="D146" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E146" s="19"/>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B147" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="C147" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="D147" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E147" s="19"/>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B148" s="21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C148" s="21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D148" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E148" s="19"/>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B149" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="C149" s="21"/>
+        <v>215</v>
+      </c>
+      <c r="C149" s="21" t="s">
+        <v>215</v>
+      </c>
       <c r="D149" s="21" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E149" s="19"/>
-      <c r="F149" s="17" t="s">
-        <v>159</v>
-      </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B150" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="C150" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="D150" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E150" s="19"/>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B151" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="C151" s="21"/>
+      <c r="D151" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E151" s="19"/>
+      <c r="F151" s="17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B152" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="C150" s="21"/>
-      <c r="D150" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E150" s="19"/>
-      <c r="F150" s="17" t="s">
+      <c r="C152" s="21"/>
+      <c r="D152" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E152" s="19"/>
+      <c r="F152" s="17" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B151" s="21"/>
-      <c r="C151" s="21" t="s">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B153" s="21"/>
+      <c r="C153" s="21" t="s">
         <v>301</v>
       </c>
-      <c r="D151" s="21" t="s">
+      <c r="D153" s="21" t="s">
         <v>338</v>
       </c>
-      <c r="E151" s="19"/>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A153" s="11" t="s">
+      <c r="E153" s="19"/>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A155" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="B153" s="25"/>
-      <c r="C153" s="25"/>
-      <c r="D153" s="25"/>
-      <c r="E153" s="35"/>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A154" s="10"/>
-      <c r="B154" s="21" t="s">
-        <v>217</v>
-      </c>
-      <c r="C154" s="21" t="s">
-        <v>217</v>
-      </c>
-      <c r="D154" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E154" s="19"/>
-      <c r="F154" s="25" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A155" s="10"/>
-      <c r="B155" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="C155" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="D155" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E155" s="19"/>
-      <c r="F155" s="18" t="s">
-        <v>263</v>
-      </c>
+      <c r="B155" s="25"/>
+      <c r="C155" s="25"/>
+      <c r="D155" s="25"/>
+      <c r="E155" s="35"/>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" s="10"/>
       <c r="B156" s="21" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C156" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="D156" s="18" t="s">
-        <v>47</v>
+        <v>217</v>
+      </c>
+      <c r="D156" s="25" t="s">
+        <v>45</v>
       </c>
       <c r="E156" s="19"/>
-      <c r="F156" s="18" t="s">
-        <v>95</v>
+      <c r="F156" s="25" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" s="10"/>
-      <c r="B157" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="C157" s="18" t="s">
-        <v>220</v>
+      <c r="B157" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="C157" s="21" t="s">
+        <v>218</v>
       </c>
       <c r="D157" s="18" t="s">
         <v>47</v>
       </c>
       <c r="E157" s="19"/>
       <c r="F157" s="18" t="s">
-        <v>93</v>
+        <v>263</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" s="10"/>
-      <c r="B158" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="C158" s="18" t="s">
-        <v>221</v>
+      <c r="B158" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="C158" s="21" t="s">
+        <v>219</v>
       </c>
       <c r="D158" s="18" t="s">
         <v>47</v>
       </c>
       <c r="E158" s="19"/>
       <c r="F158" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" s="10"/>
       <c r="B159" s="18" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C159" s="18" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D159" s="18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E159" s="19"/>
       <c r="F159" s="18" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" s="10"/>
       <c r="B160" s="18" t="s">
-        <v>177</v>
+        <v>221</v>
       </c>
       <c r="C160" s="18" t="s">
-        <v>177</v>
+        <v>221</v>
       </c>
       <c r="D160" s="18" t="s">
         <v>47</v>
       </c>
       <c r="E160" s="19"/>
       <c r="F160" s="18" t="s">
-        <v>9</v>
+        <v>94</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="10"/>
       <c r="B161" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="C161" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="D161" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E161" s="19"/>
+      <c r="F161" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A162" s="10"/>
+      <c r="B162" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C162" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="D162" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E162" s="19"/>
+      <c r="F162" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A163" s="10"/>
+      <c r="B163" s="18" t="s">
         <v>247</v>
       </c>
-      <c r="C161" s="18" t="s">
+      <c r="C163" s="18" t="s">
         <v>247</v>
       </c>
-      <c r="D161" s="18" t="s">
+      <c r="D163" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="F161" s="18" t="s">
+      <c r="F163" s="18" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C162" s="45"/>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A163" s="11" t="s">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C164" s="45"/>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A165" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="B163" s="25"/>
-      <c r="C163" s="25"/>
-      <c r="D163" s="25"/>
-      <c r="E163" s="35"/>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A164" s="10"/>
-      <c r="B164" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="C164" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="D164" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E164" s="19"/>
-      <c r="F164" s="25" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A165" s="10"/>
-      <c r="B165" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="C165" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="D165" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E165" s="19"/>
-      <c r="F165" s="18" t="s">
-        <v>263</v>
-      </c>
+      <c r="B165" s="25"/>
+      <c r="C165" s="25"/>
+      <c r="D165" s="25"/>
+      <c r="E165" s="35"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="10"/>
       <c r="B166" s="21" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C166" s="21" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D166" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E166" s="19"/>
-      <c r="F166" s="18" t="s">
-        <v>95</v>
+      <c r="F166" s="25" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="10"/>
       <c r="B167" s="21" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C167" s="21" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D167" s="21" t="s">
         <v>47</v>
       </c>
       <c r="E167" s="19"/>
       <c r="F167" s="18" t="s">
-        <v>99</v>
+        <v>263</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="10"/>
       <c r="B168" s="21" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C168" s="21" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="D168" s="21" t="s">
         <v>47</v>
       </c>
       <c r="E168" s="19"/>
       <c r="F168" s="18" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="10"/>
       <c r="B169" s="21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C169" s="21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D169" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E169" s="24"/>
+        <v>47</v>
+      </c>
+      <c r="E169" s="19"/>
       <c r="F169" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="10"/>
       <c r="B170" s="21" t="s">
-        <v>226</v>
+        <v>221</v>
+      </c>
+      <c r="C170" s="21" t="s">
+        <v>221</v>
       </c>
       <c r="D170" s="21" t="s">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="E170" s="19"/>
       <c r="F170" s="18" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="10"/>
       <c r="B171" s="21" t="s">
-        <v>177</v>
+        <v>222</v>
       </c>
       <c r="C171" s="21" t="s">
-        <v>177</v>
+        <v>222</v>
       </c>
       <c r="D171" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E171" s="19"/>
+        <v>45</v>
+      </c>
+      <c r="E171" s="24"/>
       <c r="F171" s="18" t="s">
-        <v>9</v>
+        <v>101</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" s="10"/>
       <c r="B172" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="C172" s="21" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
       <c r="D172" s="21" t="s">
-        <v>60</v>
+        <v>105</v>
       </c>
       <c r="E172" s="19"/>
       <c r="F172" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A173" s="10"/>
+      <c r="B173" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C173" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="D173" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E173" s="19"/>
+      <c r="F173" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A174" s="10"/>
+      <c r="B174" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="C174" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="D174" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E174" s="19"/>
+      <c r="F174" s="18" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B173" s="19"/>
-      <c r="C173" s="19"/>
-      <c r="D173" s="19"/>
-      <c r="E173" s="19"/>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A174" s="11" t="s">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B175" s="19"/>
+      <c r="C175" s="19"/>
+      <c r="D175" s="19"/>
+      <c r="E175" s="19"/>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A176" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="B174" s="25" t="s">
+      <c r="B176" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="C174" s="25"/>
-      <c r="D174" s="25" t="s">
+      <c r="C176" s="25"/>
+      <c r="D176" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E174" s="35"/>
-      <c r="F174" s="25" t="s">
+      <c r="E176" s="35"/>
+      <c r="F176" s="25" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B175" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="C175" s="21"/>
-      <c r="D175" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E175" s="19"/>
-      <c r="F175" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B176" s="29" t="s">
-        <v>255</v>
-      </c>
-      <c r="C176" s="29"/>
-      <c r="D176" s="29" t="s">
-        <v>256</v>
-      </c>
-      <c r="E176" s="19"/>
-      <c r="F176" s="18" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B177" s="21" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="C177" s="21"/>
-      <c r="D177" s="18" t="s">
+      <c r="D177" s="21" t="s">
         <v>47</v>
       </c>
       <c r="E177" s="19"/>
       <c r="F177" s="18" t="s">
-        <v>227</v>
+        <v>156</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B178" s="29" t="s">
-        <v>351</v>
+        <v>255</v>
       </c>
       <c r="C178" s="29"/>
-      <c r="D178" s="29"/>
+      <c r="D178" s="29" t="s">
+        <v>256</v>
+      </c>
       <c r="E178" s="19"/>
-      <c r="F178" s="18"/>
+      <c r="F178" s="18" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B179" s="21" t="s">
-        <v>259</v>
+        <v>169</v>
       </c>
       <c r="C179" s="21"/>
       <c r="D179" s="18" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E179" s="19"/>
       <c r="F179" s="18" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B180" s="29" t="s">
+        <v>351</v>
+      </c>
+      <c r="C180" s="29"/>
+      <c r="D180" s="29"/>
+      <c r="E180" s="19"/>
+      <c r="F180" s="18"/>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B181" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="C181" s="21"/>
+      <c r="D181" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E181" s="19"/>
+      <c r="F181" s="18" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B180" s="21" t="s">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B182" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="C180" s="21"/>
-      <c r="D180" s="21" t="s">
+      <c r="C182" s="21"/>
+      <c r="D182" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="E180" s="19"/>
-      <c r="F180" s="18" t="s">
+      <c r="E182" s="19"/>
+      <c r="F182" s="18" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B181" s="19"/>
-      <c r="C181" s="19"/>
-      <c r="D181" s="19"/>
-      <c r="E181" s="19"/>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A182" s="11" t="s">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B183" s="19"/>
+      <c r="C183" s="19"/>
+      <c r="D183" s="19"/>
+      <c r="E183" s="19"/>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A184" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="B182" s="25" t="s">
+      <c r="B184" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="C182" s="25"/>
-      <c r="D182" s="25" t="s">
+      <c r="C184" s="25"/>
+      <c r="D184" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E182" s="35"/>
-      <c r="F182" s="25" t="s">
+      <c r="E184" s="35"/>
+      <c r="F184" s="25" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B183" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="C183" s="21"/>
-      <c r="D183" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E183" s="19"/>
-      <c r="F183" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B184" s="29" t="s">
-        <v>257</v>
-      </c>
-      <c r="C184" s="29"/>
-      <c r="D184" s="29" t="s">
-        <v>258</v>
-      </c>
-      <c r="E184" s="19"/>
-      <c r="F184" s="18" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B185" s="21" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="C185" s="21"/>
       <c r="D185" s="18" t="s">
@@ -5006,270 +5007,269 @@
       </c>
       <c r="E185" s="19"/>
       <c r="F185" s="18" t="s">
-        <v>228</v>
+        <v>156</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B186" s="29" t="s">
-        <v>351</v>
+        <v>257</v>
       </c>
       <c r="C186" s="29"/>
-      <c r="D186" s="29"/>
+      <c r="D186" s="29" t="s">
+        <v>258</v>
+      </c>
       <c r="E186" s="19"/>
-      <c r="F186" s="18"/>
+      <c r="F186" s="18" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B187" s="21" t="s">
-        <v>260</v>
+        <v>169</v>
       </c>
       <c r="C187" s="21"/>
       <c r="D187" s="18" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E187" s="19"/>
       <c r="F187" s="18" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B188" s="29" t="s">
+        <v>351</v>
+      </c>
+      <c r="C188" s="29"/>
+      <c r="D188" s="29"/>
+      <c r="E188" s="19"/>
+      <c r="F188" s="18"/>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B189" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="C189" s="21"/>
+      <c r="D189" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E189" s="19"/>
+      <c r="F189" s="18" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B188" s="21" t="s">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B190" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="C188" s="21"/>
-      <c r="D188" s="21" t="s">
+      <c r="C190" s="21"/>
+      <c r="D190" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="E188" s="19"/>
-      <c r="F188" s="18" t="s">
+      <c r="E190" s="19"/>
+      <c r="F190" s="18" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A190" s="11" t="s">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B191" s="23"/>
+      <c r="C191" s="23"/>
+      <c r="D191" s="23"/>
+      <c r="E191" s="19"/>
+      <c r="F191" s="19"/>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A192" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="B192" s="23"/>
+      <c r="C192" s="23"/>
+      <c r="D192" s="23"/>
+      <c r="E192" s="19"/>
+      <c r="F192" s="23" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A193" s="55"/>
+      <c r="B193" s="23"/>
+      <c r="C193" s="23"/>
+      <c r="D193" s="23"/>
+      <c r="E193" s="19"/>
+      <c r="F193" s="19"/>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A194" s="55"/>
+      <c r="B194" s="23"/>
+      <c r="C194" s="23"/>
+      <c r="D194" s="23"/>
+      <c r="E194" s="19"/>
+      <c r="F194" s="19"/>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A195" s="55"/>
+      <c r="B195" s="23"/>
+      <c r="C195" s="23"/>
+      <c r="D195" s="23"/>
+      <c r="E195" s="19"/>
+      <c r="F195" s="19"/>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A197" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="B190" s="25" t="s">
+      <c r="B197" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="C190" s="25"/>
-      <c r="D190" s="25" t="s">
+      <c r="C197" s="25"/>
+      <c r="D197" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E190" s="35"/>
-      <c r="F190" s="25" t="s">
+      <c r="E197" s="35"/>
+      <c r="F197" s="25" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B191" s="21" t="s">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B198" s="21" t="s">
         <v>226</v>
-      </c>
-      <c r="C191" s="21"/>
-      <c r="D191" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E191" s="23"/>
-      <c r="F191" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B192" s="21" t="s">
-        <v>230</v>
-      </c>
-      <c r="C192" s="21"/>
-      <c r="D192" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E192" s="23"/>
-      <c r="F192" s="18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B193" s="21"/>
-      <c r="C193" s="21"/>
-      <c r="D193" s="21"/>
-      <c r="E193" s="23"/>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A195" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B195" s="25" t="s">
-        <v>231</v>
-      </c>
-      <c r="C195" s="25"/>
-      <c r="D195" s="25"/>
-      <c r="E195" s="35"/>
-      <c r="F195" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B196" s="21" t="s">
-        <v>232</v>
-      </c>
-      <c r="C196" s="21"/>
-      <c r="D196" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E196" s="23"/>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B197" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="C197" s="21"/>
-      <c r="D197" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E197" s="23"/>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B198" s="21" t="s">
-        <v>234</v>
       </c>
       <c r="C198" s="21"/>
       <c r="D198" s="21" t="s">
         <v>47</v>
       </c>
       <c r="E198" s="23"/>
-      <c r="F198" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B199" s="29" t="s">
-        <v>235</v>
-      </c>
-      <c r="C199" s="29"/>
-      <c r="D199" s="29" t="s">
+      <c r="F198" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B199" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="C199" s="21"/>
+      <c r="D199" s="21" t="s">
         <v>47</v>
       </c>
       <c r="E199" s="23"/>
-      <c r="F199" s="17" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F199" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B200" s="21"/>
       <c r="C200" s="21"/>
       <c r="D200" s="21"/>
       <c r="E200" s="23"/>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B201" s="21"/>
-      <c r="C201" s="21"/>
-      <c r="D201" s="21"/>
-      <c r="E201" s="23"/>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B202" s="21"/>
-      <c r="C202" s="21"/>
-      <c r="D202" s="21"/>
-      <c r="E202" s="23"/>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A204" s="11" t="s">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A202" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B202" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="C202" s="25"/>
+      <c r="D202" s="25"/>
+      <c r="E202" s="35"/>
+      <c r="F202" s="17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B203" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="C203" s="21"/>
+      <c r="D203" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E203" s="23"/>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B204" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="C204" s="21"/>
+      <c r="D204" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E204" s="23"/>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B205" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="C205" s="21"/>
+      <c r="D205" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E205" s="23"/>
+      <c r="F205" s="17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B206" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="C206" s="29"/>
+      <c r="D206" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E206" s="23"/>
+      <c r="F206" s="17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B207" s="21"/>
+      <c r="C207" s="21"/>
+      <c r="D207" s="21"/>
+      <c r="E207" s="23"/>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B208" s="21"/>
+      <c r="C208" s="21"/>
+      <c r="D208" s="21"/>
+      <c r="E208" s="23"/>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B209" s="21"/>
+      <c r="C209" s="21"/>
+      <c r="D209" s="21"/>
+      <c r="E209" s="23"/>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A211" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B204" s="25"/>
-      <c r="C204" s="25"/>
-      <c r="D204" s="25"/>
-      <c r="E204" s="35"/>
-      <c r="I204" s="17" t="s">
+      <c r="B211" s="25"/>
+      <c r="C211" s="25"/>
+      <c r="D211" s="25"/>
+      <c r="E211" s="35"/>
+      <c r="I211" s="17" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B205" s="21"/>
-      <c r="C205" s="21"/>
-      <c r="D205" s="21"/>
-      <c r="E205" s="23"/>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B206" s="21"/>
-      <c r="C206" s="21"/>
-      <c r="D206" s="21"/>
-      <c r="E206" s="23"/>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A208" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B208" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="C208" s="25"/>
-      <c r="D208" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E208" s="35"/>
-      <c r="F208" s="17" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B209" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="C209" s="21"/>
-      <c r="D209" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E209" s="23"/>
-    </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B210" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="C210" s="21"/>
-      <c r="D210" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E210" s="23"/>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B211" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="C211" s="29"/>
-      <c r="D211" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="E211" s="24"/>
-    </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B212" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="C212" s="18"/>
-      <c r="D212" s="21" t="s">
-        <v>47</v>
-      </c>
+      <c r="B212" s="21"/>
+      <c r="C212" s="21"/>
+      <c r="D212" s="21"/>
       <c r="E212" s="23"/>
-      <c r="F212" s="17" t="s">
-        <v>148</v>
-      </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B213" s="21" t="s">
-        <v>177</v>
-      </c>
+      <c r="B213" s="21"/>
       <c r="C213" s="21"/>
-      <c r="D213" s="18"/>
-      <c r="E213" s="19"/>
-      <c r="F213" s="17" t="s">
-        <v>135</v>
-      </c>
+      <c r="D213" s="21"/>
+      <c r="E213" s="23"/>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A215" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B215" s="25" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C215" s="25"/>
       <c r="D215" s="25" t="s">
@@ -5279,23 +5279,20 @@
       <c r="F215" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="I215" s="23" t="s">
-        <v>149</v>
-      </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B216" s="21" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="C216" s="21"/>
       <c r="D216" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E216" s="23"/>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B217" s="21" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="C217" s="21"/>
       <c r="D217" s="21" t="s">
@@ -5339,20 +5336,26 @@
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A222" s="11" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B222" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C222" s="25"/>
       <c r="D222" s="25" t="s">
         <v>45</v>
       </c>
       <c r="E222" s="35"/>
+      <c r="F222" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="I222" s="23" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B223" s="21" t="s">
-        <v>238</v>
+        <v>203</v>
       </c>
       <c r="C223" s="21"/>
       <c r="D223" s="21" t="s">
@@ -5362,7 +5365,7 @@
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B224" s="21" t="s">
-        <v>169</v>
+        <v>204</v>
       </c>
       <c r="C224" s="21"/>
       <c r="D224" s="21" t="s">
@@ -5370,178 +5373,182 @@
       </c>
       <c r="E224" s="23"/>
     </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B225" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="C225" s="29"/>
+      <c r="D225" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="E225" s="24"/>
+    </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A226" s="17"/>
-      <c r="B226" s="40" t="s">
+      <c r="B226" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="C226" s="18"/>
+      <c r="D226" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E226" s="23"/>
+      <c r="F226" s="17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B227" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C227" s="21"/>
+      <c r="D227" s="18"/>
+      <c r="E227" s="19"/>
+      <c r="F227" s="17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A229" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B229" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="C226" s="40"/>
-      <c r="D226" s="40" t="s">
+      <c r="C229" s="25"/>
+      <c r="D229" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E229" s="35"/>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B230" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="E226" s="40"/>
-      <c r="F226" s="40" t="s">
+      <c r="C230" s="21"/>
+      <c r="D230" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E230" s="23"/>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B231" s="21" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="227" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A227" s="17"/>
-      <c r="B227" s="41">
+      <c r="C231" s="21"/>
+      <c r="D231" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E231" s="23"/>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A233" s="17"/>
+      <c r="B233" s="40" t="s">
+        <v>241</v>
+      </c>
+      <c r="C233" s="40"/>
+      <c r="D233" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="E233" s="40"/>
+      <c r="F233" s="40" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A234" s="17"/>
+      <c r="B234" s="41">
         <v>1</v>
       </c>
-      <c r="C227" s="41"/>
-      <c r="D227" s="42" t="s">
+      <c r="C234" s="41"/>
+      <c r="D234" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="E227" s="42"/>
-      <c r="F227" s="42" t="s">
+      <c r="E234" s="42"/>
+      <c r="F234" s="42" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A228" s="17"/>
-      <c r="B228" s="41">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A235" s="17"/>
+      <c r="B235" s="41">
         <v>2</v>
       </c>
-      <c r="C228" s="41"/>
-      <c r="D228" s="42" t="s">
+      <c r="C235" s="41"/>
+      <c r="D235" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="E228" s="42"/>
-      <c r="F228" s="42" t="s">
+      <c r="E235" s="42"/>
+      <c r="F235" s="42" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="229" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A229" s="17"/>
-      <c r="B229" s="41">
+    <row r="236" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A236" s="17"/>
+      <c r="B236" s="41">
         <v>3</v>
       </c>
-      <c r="C229" s="41"/>
-      <c r="D229" s="42" t="s">
+      <c r="C236" s="41"/>
+      <c r="D236" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="E229" s="42"/>
-      <c r="F229" s="42" t="s">
+      <c r="E236" s="42"/>
+      <c r="F236" s="42" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A230" s="17"/>
-      <c r="B230" s="41">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A237" s="17"/>
+      <c r="B237" s="41">
         <v>4</v>
       </c>
-      <c r="C230" s="41"/>
-      <c r="D230" s="42" t="s">
+      <c r="C237" s="41"/>
+      <c r="D237" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="E230" s="42"/>
-      <c r="F230" s="42" t="s">
+      <c r="E237" s="42"/>
+      <c r="F237" s="42" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A231" s="17"/>
-      <c r="B231" s="41">
+    <row r="238" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A238" s="17"/>
+      <c r="B238" s="41">
         <v>5</v>
       </c>
-      <c r="C231" s="41"/>
-      <c r="D231" s="42" t="s">
+      <c r="C238" s="41"/>
+      <c r="D238" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="E231" s="42"/>
-      <c r="F231" s="42" t="s">
+      <c r="E238" s="42"/>
+      <c r="F238" s="42" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A232" s="17"/>
-      <c r="B232" s="41">
+    <row r="239" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A239" s="17"/>
+      <c r="B239" s="41">
         <v>6</v>
       </c>
-      <c r="C232" s="41"/>
-      <c r="D232" s="42" t="s">
+      <c r="C239" s="41"/>
+      <c r="D239" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="E232" s="42"/>
-      <c r="F232" s="42" t="s">
+      <c r="E239" s="42"/>
+      <c r="F239" s="42" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A234" s="11" t="s">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A241" s="11" t="s">
         <v>352</v>
       </c>
-      <c r="B234" s="65"/>
-      <c r="C234" s="65"/>
-      <c r="D234" s="65"/>
-    </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B235" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="C235" s="18"/>
-      <c r="D235" s="18"/>
-      <c r="E235" s="18"/>
-      <c r="F235" s="18"/>
-    </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B236" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="C236" s="18"/>
-      <c r="D236" s="18"/>
-      <c r="E236" s="18"/>
-      <c r="F236" s="18"/>
-    </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B237" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="C237" s="18"/>
-      <c r="D237" s="18"/>
-      <c r="E237" s="18"/>
-      <c r="F237" s="18"/>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B238" s="21" t="s">
-        <v>353</v>
-      </c>
-      <c r="C238" s="18"/>
-      <c r="D238" s="18"/>
-      <c r="E238" s="18"/>
-      <c r="F238" s="18"/>
-    </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B239" s="21" t="s">
-        <v>354</v>
-      </c>
-      <c r="C239" s="18"/>
-      <c r="D239" s="18"/>
-      <c r="E239" s="18"/>
-      <c r="F239" s="18"/>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B240" s="21" t="s">
-        <v>355</v>
-      </c>
-      <c r="C240" s="18"/>
-      <c r="D240" s="18"/>
-      <c r="E240" s="18"/>
-      <c r="F240" s="18"/>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B241" s="21" t="s">
-        <v>356</v>
-      </c>
-      <c r="C241" s="18"/>
-      <c r="D241" s="18"/>
-      <c r="E241" s="18"/>
-      <c r="F241" s="18"/>
+      <c r="B241" s="65"/>
+      <c r="C241" s="65"/>
+      <c r="D241" s="65"/>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B242" s="21" t="s">
-        <v>357</v>
+        <v>187</v>
       </c>
       <c r="C242" s="18"/>
       <c r="D242" s="18"/>
@@ -5550,7 +5557,7 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B243" s="21" t="s">
-        <v>358</v>
+        <v>203</v>
       </c>
       <c r="C243" s="18"/>
       <c r="D243" s="18"/>
@@ -5559,237 +5566,223 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B244" s="21" t="s">
-        <v>247</v>
+        <v>168</v>
       </c>
       <c r="C244" s="18"/>
       <c r="D244" s="18"/>
       <c r="E244" s="18"/>
       <c r="F244" s="18"/>
     </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B245" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="C245" s="18"/>
+      <c r="D245" s="18"/>
+      <c r="E245" s="18"/>
+      <c r="F245" s="18"/>
+    </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A246" s="11" t="s">
+      <c r="B246" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="C246" s="18"/>
+      <c r="D246" s="18"/>
+      <c r="E246" s="18"/>
+      <c r="F246" s="18"/>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B247" s="21" t="s">
+        <v>355</v>
+      </c>
+      <c r="C247" s="18"/>
+      <c r="D247" s="18"/>
+      <c r="E247" s="18"/>
+      <c r="F247" s="18"/>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B248" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="C248" s="18"/>
+      <c r="D248" s="18"/>
+      <c r="E248" s="18"/>
+      <c r="F248" s="18"/>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B249" s="21" t="s">
+        <v>357</v>
+      </c>
+      <c r="C249" s="18"/>
+      <c r="D249" s="18"/>
+      <c r="E249" s="18"/>
+      <c r="F249" s="18"/>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B250" s="21" t="s">
+        <v>358</v>
+      </c>
+      <c r="C250" s="18"/>
+      <c r="D250" s="18"/>
+      <c r="E250" s="18"/>
+      <c r="F250" s="18"/>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B251" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="C251" s="18"/>
+      <c r="D251" s="18"/>
+      <c r="E251" s="18"/>
+      <c r="F251" s="18"/>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A253" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="B246" s="25"/>
-      <c r="C246" s="25"/>
-      <c r="D246" s="25"/>
-      <c r="F246" s="17" t="s">
+      <c r="B253" s="25"/>
+      <c r="C253" s="25"/>
+      <c r="D253" s="25"/>
+      <c r="F253" s="17" t="s">
         <v>451</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B247" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="D247" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F247" s="17" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A248" s="72"/>
-      <c r="B248" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="D248" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="F248" s="36" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B249" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="D249" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F249" s="23" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B250" s="17" t="s">
-        <v>392</v>
-      </c>
-      <c r="D250" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F250" s="17" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B251" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="D251" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F251" s="17" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B252" s="17" t="s">
-        <v>369</v>
-      </c>
-      <c r="D252" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F252" s="17" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B253" s="17" t="s">
-        <v>370</v>
-      </c>
-      <c r="D253" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F253" s="17" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B254" s="17" t="s">
-        <v>396</v>
+        <v>187</v>
       </c>
       <c r="D254" s="17" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="F254" s="17" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B255" s="17" t="s">
-        <v>440</v>
-      </c>
-      <c r="D255" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F255" s="17" t="s">
-        <v>452</v>
+        <v>412</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A255" s="67"/>
+      <c r="B255" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="D255" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F255" s="36" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B256" s="17" t="s">
-        <v>402</v>
+        <v>247</v>
       </c>
       <c r="D256" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F256" s="17" t="s">
-        <v>423</v>
+        <v>60</v>
+      </c>
+      <c r="F256" s="23" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="257" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B257" s="17" t="s">
-        <v>413</v>
+        <v>392</v>
       </c>
       <c r="D257" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F257" s="17" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="258" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B258" s="17" t="s">
-        <v>414</v>
+        <v>393</v>
       </c>
       <c r="D258" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F258" s="17" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
     </row>
     <row r="259" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B259" s="17" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D259" s="17" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="F259" s="17" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="260" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B260" s="17" t="s">
-        <v>372</v>
-      </c>
-      <c r="D260" s="17" t="s">
-        <v>47</v>
+        <v>370</v>
+      </c>
+      <c r="D260" s="23" t="s">
+        <v>60</v>
       </c>
       <c r="F260" s="17" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="261" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B261" s="17" t="s">
-        <v>375</v>
+        <v>396</v>
       </c>
       <c r="D261" s="17" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="F261" s="17" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="262" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B262" s="17" t="s">
-        <v>376</v>
-      </c>
-      <c r="D262" s="17" t="s">
-        <v>47</v>
+        <v>440</v>
+      </c>
+      <c r="D262" s="23" t="s">
+        <v>45</v>
       </c>
       <c r="F262" s="17" t="s">
-        <v>421</v>
+        <v>452</v>
       </c>
     </row>
     <row r="263" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B263" s="17" t="s">
-        <v>379</v>
+        <v>402</v>
       </c>
       <c r="D263" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F263" s="17" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="264" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B264" s="17" t="s">
-        <v>380</v>
+        <v>413</v>
       </c>
       <c r="D264" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F264" s="17" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="265" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B265" s="17" t="s">
-        <v>381</v>
+        <v>414</v>
       </c>
       <c r="D265" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F265" s="17" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="266" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B266" s="17" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="D266" s="17" t="s">
         <v>47</v>
@@ -5800,7 +5793,7 @@
     </row>
     <row r="267" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B267" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D267" s="17" t="s">
         <v>47</v>
@@ -5811,7 +5804,7 @@
     </row>
     <row r="268" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B268" s="17" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D268" s="17" t="s">
         <v>47</v>
@@ -5822,7 +5815,7 @@
     </row>
     <row r="269" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B269" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D269" s="17" t="s">
         <v>47</v>
@@ -5833,7 +5826,7 @@
     </row>
     <row r="270" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B270" s="17" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D270" s="17" t="s">
         <v>47</v>
@@ -5844,7 +5837,7 @@
     </row>
     <row r="271" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B271" s="17" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D271" s="17" t="s">
         <v>47</v>
@@ -5855,7 +5848,7 @@
     </row>
     <row r="272" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B272" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D272" s="17" t="s">
         <v>47</v>
@@ -5864,9 +5857,9 @@
         <v>421</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="273" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B273" s="17" t="s">
-        <v>420</v>
+        <v>389</v>
       </c>
       <c r="D273" s="17" t="s">
         <v>47</v>
@@ -5875,9 +5868,9 @@
         <v>421</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="274" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B274" s="17" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="D274" s="17" t="s">
         <v>47</v>
@@ -5886,394 +5879,387 @@
         <v>421</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="275" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B275" s="17" t="s">
+        <v>374</v>
+      </c>
+      <c r="D275" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F275" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="276" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B276" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="D276" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F276" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="277" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B277" s="17" t="s">
+        <v>378</v>
+      </c>
+      <c r="D277" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F277" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="278" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B278" s="17" t="s">
+        <v>383</v>
+      </c>
+      <c r="D278" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F278" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="279" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B279" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="D279" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F279" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="280" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B280" s="17" t="s">
+        <v>420</v>
+      </c>
+      <c r="D280" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F280" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="281" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B281" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="D281" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F281" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="282" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B282" s="17" t="s">
         <v>384</v>
       </c>
-      <c r="D275" s="17" t="s">
+      <c r="D282" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F275" s="17" t="s">
+      <c r="F282" s="17" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B276" s="17" t="s">
+    <row r="283" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B283" s="17" t="s">
         <v>385</v>
       </c>
-      <c r="D276" s="17" t="s">
+      <c r="D283" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F276" s="17" t="s">
+      <c r="F283" s="17" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B277" s="17" t="s">
+    <row r="284" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B284" s="17" t="s">
         <v>386</v>
       </c>
-      <c r="D277" s="17" t="s">
+      <c r="D284" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F277" s="17" t="s">
+      <c r="F284" s="17" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B278" s="17" t="s">
+    <row r="285" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B285" s="17" t="s">
         <v>388</v>
       </c>
-      <c r="D278" s="17" t="s">
+      <c r="D285" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F278" s="17" t="s">
+      <c r="F285" s="17" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B279" s="17" t="s">
+    <row r="286" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B286" s="17" t="s">
         <v>395</v>
       </c>
-      <c r="D279" s="17" t="s">
+      <c r="D286" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F279" s="17" t="s">
+      <c r="F286" s="17" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B280" s="17" t="s">
+    <row r="287" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B287" s="17" t="s">
         <v>390</v>
       </c>
-      <c r="D280" s="17" t="s">
+      <c r="D287" s="17" t="s">
         <v>407</v>
       </c>
-      <c r="F280" s="17" t="s">
+      <c r="F287" s="17" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B281" s="17" t="s">
+    <row r="288" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B288" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="D281" s="17" t="s">
+      <c r="D288" s="17" t="s">
         <v>407</v>
       </c>
-      <c r="F281" s="17" t="s">
+      <c r="F288" s="17" t="s">
         <v>424</v>
-      </c>
-    </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B282" s="17" t="s">
-        <v>404</v>
-      </c>
-      <c r="D282" s="17" t="s">
-        <v>407</v>
-      </c>
-      <c r="F282" s="17" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B283" s="17" t="s">
-        <v>391</v>
-      </c>
-      <c r="D283" s="17" t="s">
-        <v>407</v>
-      </c>
-      <c r="F283" s="17" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B284" s="17" t="s">
-        <v>405</v>
-      </c>
-      <c r="D284" s="17" t="s">
-        <v>407</v>
-      </c>
-      <c r="F284" s="17" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B285" s="17" t="s">
-        <v>394</v>
-      </c>
-      <c r="D285" s="17" t="s">
-        <v>407</v>
-      </c>
-      <c r="F285" s="17" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A287" s="11" t="s">
-        <v>441</v>
-      </c>
-      <c r="B287" s="25"/>
-      <c r="C287" s="25"/>
-      <c r="D287" s="25"/>
-      <c r="F287" s="17" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B288" s="17" t="s">
-        <v>434</v>
-      </c>
-      <c r="D288" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F288" s="17" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B289" s="17" t="s">
-        <v>435</v>
-      </c>
-      <c r="D289" s="23" t="s">
-        <v>47</v>
+        <v>404</v>
+      </c>
+      <c r="D289" s="17" t="s">
+        <v>407</v>
       </c>
       <c r="F289" s="17" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B290" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="D290" s="23" t="s">
-        <v>45</v>
+        <v>391</v>
+      </c>
+      <c r="D290" s="17" t="s">
+        <v>407</v>
       </c>
       <c r="F290" s="17" t="s">
-        <v>412</v>
+        <v>427</v>
       </c>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B291" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="D291" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F291" s="36" t="s">
-        <v>411</v>
+        <v>405</v>
+      </c>
+      <c r="D291" s="17" t="s">
+        <v>407</v>
+      </c>
+      <c r="F291" s="17" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B292" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="D292" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F292" s="23" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B293" s="17" t="s">
-        <v>436</v>
-      </c>
-      <c r="D293" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F293" s="23" t="s">
-        <v>462</v>
+        <v>394</v>
+      </c>
+      <c r="D292" s="17" t="s">
+        <v>407</v>
+      </c>
+      <c r="F292" s="17" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B294" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="D294" s="23" t="s">
-        <v>45</v>
-      </c>
+      <c r="A294" s="11" t="s">
+        <v>441</v>
+      </c>
+      <c r="B294" s="25"/>
+      <c r="C294" s="25"/>
+      <c r="D294" s="25"/>
       <c r="F294" s="17" t="s">
-        <v>457</v>
+        <v>422</v>
       </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B295" s="17" t="s">
-        <v>369</v>
+        <v>434</v>
       </c>
       <c r="D295" s="23" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="F295" s="17" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B296" s="17" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D296" s="23" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F296" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B297" s="17" t="s">
-        <v>438</v>
+        <v>187</v>
       </c>
       <c r="D297" s="23" t="s">
         <v>45</v>
       </c>
       <c r="F297" s="17" t="s">
-        <v>461</v>
+        <v>412</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B298" s="17" t="s">
-        <v>439</v>
+        <v>203</v>
       </c>
       <c r="D298" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F298" s="17" t="s">
-        <v>459</v>
+        <v>47</v>
+      </c>
+      <c r="F298" s="36" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B299" s="17" t="s">
-        <v>440</v>
+        <v>247</v>
       </c>
       <c r="D299" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F299" s="17" t="s">
-        <v>452</v>
+        <v>60</v>
+      </c>
+      <c r="F299" s="23" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A300" s="17"/>
       <c r="B300" s="17" t="s">
-        <v>402</v>
+        <v>436</v>
       </c>
       <c r="D300" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F300" s="17" t="s">
-        <v>423</v>
+        <v>60</v>
+      </c>
+      <c r="F300" s="23" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A301" s="17"/>
       <c r="B301" s="17" t="s">
-        <v>413</v>
+        <v>223</v>
       </c>
       <c r="D301" s="23" t="s">
         <v>45</v>
       </c>
       <c r="F301" s="17" t="s">
-        <v>415</v>
+        <v>457</v>
       </c>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A302" s="17"/>
       <c r="B302" s="17" t="s">
-        <v>414</v>
+        <v>369</v>
       </c>
       <c r="D302" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F302" s="17" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B303" s="17" t="s">
+        <v>437</v>
+      </c>
+      <c r="D303" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F302" s="17" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A303" s="17"/>
-      <c r="B303" s="17" t="s">
-        <v>371</v>
-      </c>
-      <c r="D303" s="23" t="s">
-        <v>47</v>
-      </c>
       <c r="F303" s="17" t="s">
-        <v>421</v>
+        <v>460</v>
       </c>
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A304" s="17"/>
       <c r="B304" s="17" t="s">
-        <v>372</v>
+        <v>438</v>
       </c>
       <c r="D304" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F304" s="17" t="s">
-        <v>421</v>
+        <v>461</v>
       </c>
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A305" s="17"/>
       <c r="B305" s="17" t="s">
-        <v>375</v>
+        <v>439</v>
       </c>
       <c r="D305" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F305" s="17" t="s">
-        <v>421</v>
+        <v>459</v>
       </c>
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A306" s="17"/>
       <c r="B306" s="17" t="s">
-        <v>376</v>
+        <v>440</v>
       </c>
       <c r="D306" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F306" s="17" t="s">
-        <v>421</v>
+        <v>452</v>
       </c>
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A307" s="17"/>
       <c r="B307" s="17" t="s">
-        <v>379</v>
+        <v>402</v>
       </c>
       <c r="D307" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F307" s="17" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A308" s="17"/>
       <c r="B308" s="17" t="s">
-        <v>380</v>
+        <v>413</v>
       </c>
       <c r="D308" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F308" s="17" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A309" s="17"/>
       <c r="B309" s="17" t="s">
-        <v>381</v>
+        <v>414</v>
       </c>
       <c r="D309" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F309" s="17" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A310" s="17"/>
       <c r="B310" s="17" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="D310" s="23" t="s">
         <v>47</v>
@@ -6285,7 +6271,7 @@
     <row r="311" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A311" s="17"/>
       <c r="B311" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D311" s="23" t="s">
         <v>47</v>
@@ -6297,7 +6283,7 @@
     <row r="312" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A312" s="17"/>
       <c r="B312" s="17" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D312" s="23" t="s">
         <v>47</v>
@@ -6309,7 +6295,7 @@
     <row r="313" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A313" s="17"/>
       <c r="B313" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D313" s="23" t="s">
         <v>47</v>
@@ -6321,7 +6307,7 @@
     <row r="314" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A314" s="17"/>
       <c r="B314" s="17" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D314" s="23" t="s">
         <v>47</v>
@@ -6333,7 +6319,7 @@
     <row r="315" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A315" s="17"/>
       <c r="B315" s="17" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D315" s="23" t="s">
         <v>47</v>
@@ -6345,7 +6331,7 @@
     <row r="316" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A316" s="17"/>
       <c r="B316" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D316" s="23" t="s">
         <v>47</v>
@@ -6357,7 +6343,7 @@
     <row r="317" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A317" s="17"/>
       <c r="B317" s="17" t="s">
-        <v>420</v>
+        <v>389</v>
       </c>
       <c r="D317" s="23" t="s">
         <v>47</v>
@@ -6369,7 +6355,7 @@
     <row r="318" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A318" s="17"/>
       <c r="B318" s="17" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="D318" s="23" t="s">
         <v>47</v>
@@ -6381,264 +6367,404 @@
     <row r="319" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A319" s="17"/>
       <c r="B319" s="17" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="D319" s="23" t="s">
         <v>47</v>
       </c>
       <c r="F319" s="17" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A320" s="17"/>
       <c r="B320" s="17" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D320" s="23" t="s">
         <v>47</v>
       </c>
       <c r="F320" s="17" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A321" s="17"/>
       <c r="B321" s="17" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="D321" s="23" t="s">
         <v>47</v>
       </c>
       <c r="F321" s="17" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A322" s="17"/>
       <c r="B322" s="17" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="D322" s="23" t="s">
         <v>47</v>
       </c>
       <c r="F322" s="17" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A323" s="17"/>
       <c r="B323" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="D323" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F323" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A324" s="17"/>
+      <c r="B324" s="17" t="s">
+        <v>420</v>
+      </c>
+      <c r="D324" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F324" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A325" s="17"/>
+      <c r="B325" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="D325" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F325" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A326" s="17"/>
+      <c r="B326" s="17" t="s">
+        <v>384</v>
+      </c>
+      <c r="D326" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F326" s="17" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A327" s="17"/>
+      <c r="B327" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="D327" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F327" s="17" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A328" s="17"/>
+      <c r="B328" s="17" t="s">
+        <v>386</v>
+      </c>
+      <c r="D328" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F328" s="17" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A329" s="17"/>
+      <c r="B329" s="17" t="s">
+        <v>388</v>
+      </c>
+      <c r="D329" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F329" s="17" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A330" s="17"/>
+      <c r="B330" s="17" t="s">
         <v>395</v>
       </c>
-      <c r="D323" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F323" s="17" t="s">
+      <c r="D330" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F330" s="17" t="s">
         <v>433</v>
-      </c>
-    </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B324" s="17" t="s">
-        <v>390</v>
-      </c>
-      <c r="D324" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F324" s="17" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B325" s="17" t="s">
-        <v>403</v>
-      </c>
-      <c r="D325" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F325" s="17" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B326" s="17" t="s">
-        <v>404</v>
-      </c>
-      <c r="D326" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F326" s="17" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B327" s="17" t="s">
-        <v>391</v>
-      </c>
-      <c r="D327" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F327" s="17" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B328" s="17" t="s">
-        <v>394</v>
-      </c>
-      <c r="D328" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F328" s="17" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A330" s="11" t="s">
-        <v>449</v>
-      </c>
-      <c r="B330" s="25"/>
-      <c r="C330" s="25"/>
-      <c r="D330" s="25"/>
-      <c r="F330" s="17" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B331" s="17" t="s">
-        <v>434</v>
+        <v>390</v>
+      </c>
+      <c r="D331" s="23" t="s">
+        <v>47</v>
       </c>
       <c r="F331" s="17" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B332" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="F332" s="23" t="s">
-        <v>456</v>
+        <v>403</v>
+      </c>
+      <c r="D332" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F332" s="17" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B333" s="17" t="s">
-        <v>442</v>
-      </c>
-      <c r="F333" s="23" t="s">
-        <v>463</v>
+        <v>404</v>
+      </c>
+      <c r="D333" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F333" s="17" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B334" s="17" t="s">
-        <v>392</v>
-      </c>
-      <c r="F334" s="23" t="s">
-        <v>464</v>
+        <v>391</v>
+      </c>
+      <c r="D334" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F334" s="17" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B335" s="17" t="s">
+        <v>394</v>
+      </c>
+      <c r="D335" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F335" s="17" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A337" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="B337" s="25"/>
+      <c r="C337" s="25"/>
+      <c r="D337" s="25"/>
+      <c r="F337" s="17" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B338" s="17" t="s">
+        <v>434</v>
+      </c>
+      <c r="D338" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F338" s="17" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B339" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="D339" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F339" s="23" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B340" s="17" t="s">
+        <v>442</v>
+      </c>
+      <c r="D340" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F340" s="23" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B341" s="17" t="s">
+        <v>392</v>
+      </c>
+      <c r="D341" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F341" s="23" t="s">
+        <v>464</v>
+      </c>
+      <c r="G341" s="23"/>
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B342" s="17" t="s">
         <v>393</v>
       </c>
-      <c r="F335" s="23" t="s">
+      <c r="D342" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F342" s="23" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B336" s="17" t="s">
+      <c r="G342" s="23"/>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B343" s="17" t="s">
         <v>443</v>
       </c>
-      <c r="F336" s="23" t="s">
+      <c r="D343" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F343" s="23" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="337" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B337" s="17" t="s">
+      <c r="G343" s="23"/>
+    </row>
+    <row r="344" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B344" s="17" t="s">
         <v>444</v>
       </c>
-      <c r="F337" s="23" t="s">
+      <c r="D344" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F344" s="23" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="338" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B338" s="17" t="s">
+      <c r="G344" s="23"/>
+    </row>
+    <row r="345" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B345" s="17" t="s">
         <v>445</v>
       </c>
-      <c r="F338" s="23" t="s">
+      <c r="D345" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F345" s="23" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="339" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B339" s="17" t="s">
+      <c r="G345" s="23"/>
+    </row>
+    <row r="346" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B346" s="17" t="s">
         <v>446</v>
       </c>
-      <c r="F339" s="23" t="s">
+      <c r="D346" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F346" s="23" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="340" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B340" s="17" t="s">
+      <c r="G346" s="23"/>
+    </row>
+    <row r="347" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B347" s="17" t="s">
         <v>447</v>
       </c>
-      <c r="F340" s="23" t="s">
+      <c r="D347" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F347" s="23" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="341" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B341" s="17" t="s">
+      <c r="G347" s="23"/>
+    </row>
+    <row r="348" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B348" s="17" t="s">
         <v>448</v>
       </c>
-      <c r="F341" s="23" t="s">
+      <c r="D348" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F348" s="23" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="342" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B342" s="17" t="s">
+      <c r="G348" s="23"/>
+    </row>
+    <row r="349" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B349" s="17" t="s">
         <v>390</v>
       </c>
-      <c r="F342" s="17" t="s">
+      <c r="D349" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F349" s="17" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="343" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B343" s="17" t="s">
+    <row r="350" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B350" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="F343" s="17" t="s">
+      <c r="D350" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F350" s="17" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="344" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B344" s="17" t="s">
+    <row r="351" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B351" s="17" t="s">
         <v>404</v>
       </c>
-      <c r="F344" s="17" t="s">
+      <c r="D351" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F351" s="17" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="345" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B345" s="17" t="s">
+    <row r="352" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B352" s="17" t="s">
         <v>391</v>
       </c>
-      <c r="F345" s="17" t="s">
+      <c r="D352" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F352" s="17" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="346" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B346" s="17" t="s">
+    <row r="353" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B353" s="17" t="s">
         <v>394</v>
       </c>
-      <c r="F346" s="17" t="s">
+      <c r="D353" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F353" s="17" t="s">
         <v>408</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="I124:I136"/>
+    <mergeCell ref="I126:I138"/>
     <mergeCell ref="F42:H42"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J140" r:id="rId1" xr:uid="{C542003A-DE46-4D98-A11B-9CC195E7F11A}"/>
+    <hyperlink ref="J142" r:id="rId1" xr:uid="{C542003A-DE46-4D98-A11B-9CC195E7F11A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="90" r:id="rId2"/>
@@ -6650,8 +6776,8 @@
   <dimension ref="A1:N240"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B156" sqref="B156"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
NOBUG: Updating model and dataset docs (#180)
</commit_message>
<xml_diff>
--- a/docs/BC Parks CMS Data Model.xlsx
+++ b/docs/BC Parks CMS Data Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rofiddle\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF999796-8CFD-4F11-925D-6DA14C516D60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5F4106-D3EE-4866-83D5-9C5D13FDE2E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A33082D8-1C98-4870-8924-9924FABEACC5}"/>
+    <workbookView xWindow="-21825" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{A33082D8-1C98-4870-8924-9924FABEACC5}"/>
   </bookViews>
   <sheets>
     <sheet name="BCParks" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="475">
   <si>
     <t>Table</t>
   </si>
@@ -1694,12 +1694,21 @@
   <si>
     <t>Indicates the date/time that the off-season ends</t>
   </si>
+  <si>
+    <t>ParkFees</t>
+  </si>
+  <si>
+    <t>Relates to a park activity or facility</t>
+  </si>
+  <si>
+    <t>Link to ParkFeatures</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1"/>
@@ -1875,11 +1884,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="11">
@@ -2085,7 +2089,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2186,8 +2190,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2200,7 +2204,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" customBuiltin="1"/>
@@ -2522,11 +2525,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9256A4-85B0-483D-ABA5-01E16592AE65}">
-  <dimension ref="A1:J346"/>
+  <dimension ref="A1:J353"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C264" sqref="C264"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2812,7 +2815,7 @@
     </row>
     <row r="15" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="38" t="s">
         <v>169</v>
       </c>
       <c r="C15" s="38" t="s">
@@ -2821,7 +2824,7 @@
       <c r="D15" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="44" t="b">
+      <c r="E15" s="21" t="b">
         <v>0</v>
       </c>
       <c r="F15" s="21" t="s">
@@ -2830,7 +2833,7 @@
     </row>
     <row r="16" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="38" t="s">
         <v>361</v>
       </c>
       <c r="C16" s="27" t="s">
@@ -3969,7 +3972,7 @@
       <c r="I101" s="18"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A102" s="67"/>
+      <c r="A102" s="66"/>
       <c r="B102" s="29" t="s">
         <v>399</v>
       </c>
@@ -3982,95 +3985,88 @@
         <v>401</v>
       </c>
     </row>
-    <row r="103" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="4"/>
-      <c r="B103" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="C103" s="18"/>
-      <c r="D103" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E103" s="18"/>
-      <c r="F103" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="G103" s="18"/>
-      <c r="H103" s="18"/>
-      <c r="I103" s="18"/>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" s="66"/>
+      <c r="B103" s="29" t="s">
+        <v>441</v>
+      </c>
+      <c r="C103" s="21"/>
+      <c r="D103" s="20" t="s">
+        <v>474</v>
+      </c>
+      <c r="E103" s="23"/>
+      <c r="F103" s="36"/>
     </row>
     <row r="104" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4"/>
       <c r="B104" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="C104" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="D104" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="C104" s="18"/>
+      <c r="D104" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E104" s="20"/>
+      <c r="E104" s="18"/>
       <c r="F104" s="21" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="G104" s="18"/>
       <c r="H104" s="18"/>
       <c r="I104" s="18"/>
     </row>
-    <row r="105" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="6"/>
+    <row r="105" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="4"/>
       <c r="B105" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="C105" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="C105" s="18" t="s">
+        <v>272</v>
+      </c>
       <c r="D105" s="20" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E105" s="20"/>
-      <c r="F105" s="18"/>
+      <c r="F105" s="21" t="s">
+        <v>90</v>
+      </c>
       <c r="G105" s="18"/>
       <c r="H105" s="18"/>
       <c r="I105" s="18"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C106" s="23"/>
-      <c r="D106" s="36"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A108" s="11" t="s">
+    <row r="106" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="6"/>
+      <c r="B106" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="C106" s="18"/>
+      <c r="D106" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E106" s="20"/>
+      <c r="F106" s="18"/>
+      <c r="G106" s="18"/>
+      <c r="H106" s="18"/>
+      <c r="I106" s="18"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C107" s="23"/>
+      <c r="D107" s="36"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A109" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B108" s="25"/>
-      <c r="C108" s="25"/>
-      <c r="D108" s="25"/>
-      <c r="E108" s="35"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B109" s="21" t="s">
+      <c r="B109" s="25"/>
+      <c r="C109" s="25"/>
+      <c r="D109" s="25"/>
+      <c r="E109" s="35"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B110" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="C109" s="21" t="s">
+      <c r="C110" s="21" t="s">
         <v>203</v>
-      </c>
-      <c r="D109" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E109" s="23"/>
-      <c r="F109" s="36"/>
-      <c r="G109" s="36"/>
-      <c r="H109" s="36"/>
-      <c r="I109" s="36" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A110" s="17"/>
-      <c r="B110" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="C110" s="21" t="s">
-        <v>204</v>
       </c>
       <c r="D110" s="21" t="s">
         <v>47</v>
@@ -4079,17 +4075,20 @@
       <c r="F110" s="36"/>
       <c r="G110" s="36"/>
       <c r="H110" s="36"/>
-      <c r="I110" s="36"/>
+      <c r="I110" s="36" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" s="17"/>
       <c r="B111" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C111" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D111" s="21" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E111" s="23"/>
       <c r="F111" s="36"/>
@@ -4099,13 +4098,13 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B112" s="21" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C112" s="21" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="D112" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E112" s="23"/>
       <c r="F112" s="36"/>
@@ -4115,28 +4114,26 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B113" s="21" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C113" s="21" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D113" s="21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E113" s="23"/>
       <c r="F113" s="36"/>
       <c r="G113" s="36"/>
       <c r="H113" s="36"/>
-      <c r="I113" s="36" t="s">
-        <v>62</v>
-      </c>
+      <c r="I113" s="36"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B114" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C114" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D114" s="21" t="s">
         <v>46</v>
@@ -4151,34 +4148,40 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B115" s="21" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="C115" s="21" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="D115" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E115" s="19"/>
+        <v>46</v>
+      </c>
+      <c r="E115" s="23"/>
+      <c r="F115" s="36"/>
+      <c r="G115" s="36"/>
+      <c r="H115" s="36"/>
+      <c r="I115" s="36" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B116" s="21" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="C116" s="21" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="D116" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E116" s="19"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B117" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C117" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D117" s="21" t="s">
         <v>48</v>
@@ -4187,818 +4190,816 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B118" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C118" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D118" s="21" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E118" s="19"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B119" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="C119" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="D119" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E119" s="19"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B120" s="21" t="s">
         <v>349</v>
       </c>
-      <c r="C119" s="21"/>
-      <c r="D119" s="21" t="s">
+      <c r="C120" s="21"/>
+      <c r="D120" s="21" t="s">
         <v>60</v>
-      </c>
-      <c r="E119" s="23"/>
-      <c r="F119" s="36" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A120" s="67"/>
-      <c r="B120" s="29" t="s">
-        <v>399</v>
-      </c>
-      <c r="C120" s="21"/>
-      <c r="D120" s="20" t="s">
-        <v>400</v>
       </c>
       <c r="E120" s="23"/>
       <c r="F120" s="36" t="s">
-        <v>401</v>
+        <v>79</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B121" s="21" t="s">
-        <v>177</v>
+      <c r="A121" s="66"/>
+      <c r="B121" s="29" t="s">
+        <v>399</v>
       </c>
       <c r="C121" s="21"/>
-      <c r="D121" s="21" t="s">
-        <v>47</v>
+      <c r="D121" s="20" t="s">
+        <v>400</v>
       </c>
       <c r="E121" s="23"/>
       <c r="F121" s="36" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A122" s="66"/>
+      <c r="B122" s="29" t="s">
+        <v>441</v>
+      </c>
+      <c r="C122" s="21"/>
+      <c r="D122" s="20" t="s">
+        <v>474</v>
+      </c>
+      <c r="E122" s="23"/>
+      <c r="F122" s="36"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B123" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C123" s="21"/>
+      <c r="D123" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E123" s="23"/>
+      <c r="F123" s="36" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B122" s="21"/>
-      <c r="C122" s="21" t="s">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B124" s="21"/>
+      <c r="C124" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="D122" s="21" t="s">
+      <c r="D124" s="21" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C123" s="45"/>
-      <c r="D123" s="56"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A124" s="11" t="s">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C125" s="45"/>
+      <c r="D125" s="56"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A126" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B124" s="25"/>
-      <c r="C124" s="25"/>
-      <c r="D124" s="25"/>
-      <c r="E124" s="35"/>
-      <c r="H124" s="17" t="s">
+      <c r="B126" s="25"/>
+      <c r="C126" s="25"/>
+      <c r="D126" s="25"/>
+      <c r="E126" s="35"/>
+      <c r="H126" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="I124" s="68" t="s">
+      <c r="I126" s="68" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A125" s="55"/>
-      <c r="B125" s="21" t="s">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A127" s="55"/>
+      <c r="B127" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="C125" s="21" t="s">
+      <c r="C127" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="D125" s="21" t="s">
+      <c r="D127" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E125" s="35"/>
-      <c r="I125" s="68"/>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B126" s="21" t="s">
+      <c r="E127" s="35"/>
+      <c r="I127" s="68"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B128" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="C126" s="21" t="s">
+      <c r="C128" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="D126" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E126" s="19"/>
-      <c r="I126" s="68"/>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B127" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C127" s="21" t="s">
-        <v>327</v>
-      </c>
-      <c r="D127" s="21"/>
-      <c r="E127" s="19"/>
-      <c r="F127" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I127" s="68"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B128" s="21"/>
-      <c r="C128" s="21" t="s">
-        <v>320</v>
-      </c>
       <c r="D128" s="21" t="s">
-        <v>338</v>
+        <v>47</v>
       </c>
       <c r="E128" s="19"/>
       <c r="I128" s="68"/>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B129" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C129" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="D129" s="21"/>
+      <c r="E129" s="19"/>
+      <c r="F129" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="I129" s="68"/>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A130" s="11" t="s">
+      <c r="B130" s="21"/>
+      <c r="C130" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="D130" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="E130" s="19"/>
+      <c r="I130" s="68"/>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I131" s="68"/>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A132" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B130" s="25"/>
-      <c r="C130" s="25"/>
-      <c r="D130" s="25" t="s">
+      <c r="B132" s="25"/>
+      <c r="C132" s="25"/>
+      <c r="D132" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E130" s="35"/>
-      <c r="H130" s="17" t="s">
+      <c r="E132" s="35"/>
+      <c r="H132" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="I130" s="68"/>
-    </row>
-    <row r="131" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="B131" s="21" t="s">
+      <c r="I132" s="68"/>
+    </row>
+    <row r="133" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="B133" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="C131" s="21" t="s">
+      <c r="C133" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="D131" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E131" s="19"/>
-      <c r="I131" s="68"/>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B132" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="C132" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D132" s="21"/>
-      <c r="E132" s="19"/>
-      <c r="F132" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="I132" s="68"/>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B133" s="21"/>
-      <c r="C133" s="21" t="s">
-        <v>311</v>
-      </c>
-      <c r="D133" s="21"/>
+      <c r="D133" s="21" t="s">
+        <v>47</v>
+      </c>
       <c r="E133" s="19"/>
       <c r="I133" s="68"/>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B134" s="21" t="s">
-        <v>25</v>
+        <v>209</v>
       </c>
       <c r="C134" s="21" t="s">
-        <v>320</v>
+        <v>209</v>
       </c>
       <c r="D134" s="21"/>
       <c r="E134" s="19"/>
+      <c r="F134" s="17" t="s">
+        <v>30</v>
+      </c>
       <c r="I134" s="68"/>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B135" s="54"/>
-      <c r="C135" s="54"/>
-      <c r="D135" s="54"/>
+      <c r="B135" s="21"/>
+      <c r="C135" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="D135" s="21"/>
       <c r="E135" s="19"/>
       <c r="I135" s="68"/>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H136" s="17" t="s">
+      <c r="B136" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C136" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="D136" s="21"/>
+      <c r="E136" s="19"/>
+      <c r="I136" s="68"/>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B137" s="54"/>
+      <c r="C137" s="54"/>
+      <c r="D137" s="54"/>
+      <c r="E137" s="19"/>
+      <c r="I137" s="68"/>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H138" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="I136" s="68"/>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A137" s="11" t="s">
+      <c r="I138" s="68"/>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A139" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B137" s="25" t="s">
+      <c r="B139" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="C137" s="25"/>
-      <c r="D137" s="25" t="s">
+      <c r="C139" s="25"/>
+      <c r="D139" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E137" s="35"/>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B138" s="38" t="s">
+      <c r="E139" s="35"/>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B140" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="C138" s="38"/>
-      <c r="D138" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E138" s="19"/>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A140" s="11" t="s">
+      <c r="C140" s="38"/>
+      <c r="D140" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E140" s="19"/>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A142" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B140" s="11"/>
-      <c r="C140" s="11"/>
-      <c r="D140" s="11"/>
-      <c r="E140" s="35"/>
-      <c r="F140" s="17" t="s">
+      <c r="B142" s="11"/>
+      <c r="C142" s="11"/>
+      <c r="D142" s="11"/>
+      <c r="E142" s="35"/>
+      <c r="F142" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="H140" s="17" t="s">
+      <c r="H142" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="J140" s="39" t="s">
+      <c r="J142" s="39" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B141" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="C141" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="D141" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E141" s="19"/>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B142" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="C142" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="D142" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E142" s="19"/>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B143" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="C143" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="D143" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E143" s="19"/>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B144" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="C144" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="D144" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E144" s="19"/>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B145" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="C143" s="21" t="s">
+      <c r="C145" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="D143" s="21"/>
-      <c r="E143" s="19"/>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A145" s="11" t="s">
+      <c r="D145" s="21"/>
+      <c r="E145" s="19"/>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A147" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B145" s="11"/>
-      <c r="C145" s="11"/>
-      <c r="D145" s="11"/>
-      <c r="E145" s="35"/>
-      <c r="F145" s="17" t="s">
+      <c r="B147" s="11"/>
+      <c r="C147" s="11"/>
+      <c r="D147" s="11"/>
+      <c r="E147" s="35"/>
+      <c r="F147" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="H145" s="17" t="s">
+      <c r="H147" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="I145" s="23" t="s">
+      <c r="I147" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="J145" s="22" t="s">
+      <c r="J147" s="22" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B146" s="21" t="s">
-        <v>214</v>
-      </c>
-      <c r="C146" s="21" t="s">
-        <v>214</v>
-      </c>
-      <c r="D146" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E146" s="19"/>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B147" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="C147" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="D147" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E147" s="19"/>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B148" s="21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C148" s="21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D148" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E148" s="19"/>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B149" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="C149" s="21"/>
+        <v>215</v>
+      </c>
+      <c r="C149" s="21" t="s">
+        <v>215</v>
+      </c>
       <c r="D149" s="21" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E149" s="19"/>
-      <c r="F149" s="17" t="s">
-        <v>159</v>
-      </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B150" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="C150" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="D150" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E150" s="19"/>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B151" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="C151" s="21"/>
+      <c r="D151" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E151" s="19"/>
+      <c r="F151" s="17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B152" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="C150" s="21"/>
-      <c r="D150" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E150" s="19"/>
-      <c r="F150" s="17" t="s">
+      <c r="C152" s="21"/>
+      <c r="D152" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E152" s="19"/>
+      <c r="F152" s="17" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B151" s="21"/>
-      <c r="C151" s="21" t="s">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B153" s="21"/>
+      <c r="C153" s="21" t="s">
         <v>301</v>
       </c>
-      <c r="D151" s="21" t="s">
+      <c r="D153" s="21" t="s">
         <v>338</v>
       </c>
-      <c r="E151" s="19"/>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A153" s="11" t="s">
+      <c r="E153" s="19"/>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A155" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="B153" s="25"/>
-      <c r="C153" s="25"/>
-      <c r="D153" s="25"/>
-      <c r="E153" s="35"/>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A154" s="10"/>
-      <c r="B154" s="21" t="s">
-        <v>217</v>
-      </c>
-      <c r="C154" s="21" t="s">
-        <v>217</v>
-      </c>
-      <c r="D154" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E154" s="19"/>
-      <c r="F154" s="25" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A155" s="10"/>
-      <c r="B155" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="C155" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="D155" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E155" s="19"/>
-      <c r="F155" s="18" t="s">
-        <v>263</v>
-      </c>
+      <c r="B155" s="25"/>
+      <c r="C155" s="25"/>
+      <c r="D155" s="25"/>
+      <c r="E155" s="35"/>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" s="10"/>
       <c r="B156" s="21" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C156" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="D156" s="18" t="s">
-        <v>47</v>
+        <v>217</v>
+      </c>
+      <c r="D156" s="25" t="s">
+        <v>45</v>
       </c>
       <c r="E156" s="19"/>
-      <c r="F156" s="18" t="s">
-        <v>95</v>
+      <c r="F156" s="25" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" s="10"/>
-      <c r="B157" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="C157" s="18" t="s">
-        <v>220</v>
+      <c r="B157" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="C157" s="21" t="s">
+        <v>218</v>
       </c>
       <c r="D157" s="18" t="s">
         <v>47</v>
       </c>
       <c r="E157" s="19"/>
       <c r="F157" s="18" t="s">
-        <v>93</v>
+        <v>263</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" s="10"/>
-      <c r="B158" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="C158" s="18" t="s">
-        <v>221</v>
+      <c r="B158" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="C158" s="21" t="s">
+        <v>219</v>
       </c>
       <c r="D158" s="18" t="s">
         <v>47</v>
       </c>
       <c r="E158" s="19"/>
       <c r="F158" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" s="10"/>
       <c r="B159" s="18" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C159" s="18" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D159" s="18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E159" s="19"/>
       <c r="F159" s="18" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" s="10"/>
       <c r="B160" s="18" t="s">
-        <v>177</v>
+        <v>221</v>
       </c>
       <c r="C160" s="18" t="s">
-        <v>177</v>
+        <v>221</v>
       </c>
       <c r="D160" s="18" t="s">
         <v>47</v>
       </c>
       <c r="E160" s="19"/>
       <c r="F160" s="18" t="s">
-        <v>9</v>
+        <v>94</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="10"/>
       <c r="B161" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="C161" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="D161" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E161" s="19"/>
+      <c r="F161" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A162" s="10"/>
+      <c r="B162" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C162" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="D162" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E162" s="19"/>
+      <c r="F162" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A163" s="10"/>
+      <c r="B163" s="18" t="s">
         <v>247</v>
       </c>
-      <c r="C161" s="18" t="s">
+      <c r="C163" s="18" t="s">
         <v>247</v>
       </c>
-      <c r="D161" s="18" t="s">
+      <c r="D163" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="F161" s="18" t="s">
+      <c r="F163" s="18" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C162" s="45"/>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A163" s="11" t="s">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C164" s="45"/>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A165" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="B163" s="25"/>
-      <c r="C163" s="25"/>
-      <c r="D163" s="25"/>
-      <c r="E163" s="35"/>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A164" s="10"/>
-      <c r="B164" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="C164" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="D164" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E164" s="19"/>
-      <c r="F164" s="25" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A165" s="10"/>
-      <c r="B165" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="C165" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="D165" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E165" s="19"/>
-      <c r="F165" s="18" t="s">
-        <v>263</v>
-      </c>
+      <c r="B165" s="25"/>
+      <c r="C165" s="25"/>
+      <c r="D165" s="25"/>
+      <c r="E165" s="35"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="10"/>
       <c r="B166" s="21" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C166" s="21" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D166" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E166" s="19"/>
-      <c r="F166" s="18" t="s">
-        <v>95</v>
+      <c r="F166" s="25" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="10"/>
       <c r="B167" s="21" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C167" s="21" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D167" s="21" t="s">
         <v>47</v>
       </c>
       <c r="E167" s="19"/>
       <c r="F167" s="18" t="s">
-        <v>99</v>
+        <v>263</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="10"/>
       <c r="B168" s="21" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C168" s="21" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="D168" s="21" t="s">
         <v>47</v>
       </c>
       <c r="E168" s="19"/>
       <c r="F168" s="18" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="10"/>
       <c r="B169" s="21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C169" s="21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D169" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E169" s="24"/>
+        <v>47</v>
+      </c>
+      <c r="E169" s="19"/>
       <c r="F169" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="10"/>
       <c r="B170" s="21" t="s">
-        <v>226</v>
+        <v>221</v>
+      </c>
+      <c r="C170" s="21" t="s">
+        <v>221</v>
       </c>
       <c r="D170" s="21" t="s">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="E170" s="19"/>
       <c r="F170" s="18" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="10"/>
       <c r="B171" s="21" t="s">
-        <v>177</v>
+        <v>222</v>
       </c>
       <c r="C171" s="21" t="s">
-        <v>177</v>
+        <v>222</v>
       </c>
       <c r="D171" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E171" s="19"/>
+        <v>45</v>
+      </c>
+      <c r="E171" s="24"/>
       <c r="F171" s="18" t="s">
-        <v>9</v>
+        <v>101</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" s="10"/>
       <c r="B172" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="C172" s="21" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
       <c r="D172" s="21" t="s">
-        <v>60</v>
+        <v>105</v>
       </c>
       <c r="E172" s="19"/>
       <c r="F172" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A173" s="10"/>
+      <c r="B173" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C173" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="D173" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E173" s="19"/>
+      <c r="F173" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A174" s="10"/>
+      <c r="B174" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="C174" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="D174" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E174" s="19"/>
+      <c r="F174" s="18" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B173" s="19"/>
-      <c r="C173" s="19"/>
-      <c r="D173" s="19"/>
-      <c r="E173" s="19"/>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A174" s="11" t="s">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B175" s="19"/>
+      <c r="C175" s="19"/>
+      <c r="D175" s="19"/>
+      <c r="E175" s="19"/>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A176" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="B174" s="25" t="s">
+      <c r="B176" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="C174" s="25"/>
-      <c r="D174" s="25" t="s">
+      <c r="C176" s="25"/>
+      <c r="D176" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E174" s="35"/>
-      <c r="F174" s="25" t="s">
+      <c r="E176" s="35"/>
+      <c r="F176" s="25" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B175" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="C175" s="21"/>
-      <c r="D175" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E175" s="19"/>
-      <c r="F175" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B176" s="29" t="s">
-        <v>255</v>
-      </c>
-      <c r="C176" s="29"/>
-      <c r="D176" s="29" t="s">
-        <v>256</v>
-      </c>
-      <c r="E176" s="19"/>
-      <c r="F176" s="18" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B177" s="21" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="C177" s="21"/>
-      <c r="D177" s="18" t="s">
+      <c r="D177" s="21" t="s">
         <v>47</v>
       </c>
       <c r="E177" s="19"/>
       <c r="F177" s="18" t="s">
-        <v>227</v>
+        <v>156</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B178" s="29" t="s">
-        <v>351</v>
+        <v>255</v>
       </c>
       <c r="C178" s="29"/>
-      <c r="D178" s="29"/>
+      <c r="D178" s="29" t="s">
+        <v>256</v>
+      </c>
       <c r="E178" s="19"/>
-      <c r="F178" s="18"/>
+      <c r="F178" s="18" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B179" s="21" t="s">
-        <v>259</v>
+        <v>169</v>
       </c>
       <c r="C179" s="21"/>
       <c r="D179" s="18" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E179" s="19"/>
       <c r="F179" s="18" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B180" s="29" t="s">
+        <v>351</v>
+      </c>
+      <c r="C180" s="29"/>
+      <c r="D180" s="29"/>
+      <c r="E180" s="19"/>
+      <c r="F180" s="18"/>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B181" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="C181" s="21"/>
+      <c r="D181" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E181" s="19"/>
+      <c r="F181" s="18" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B180" s="21" t="s">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B182" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="C180" s="21"/>
-      <c r="D180" s="21" t="s">
+      <c r="C182" s="21"/>
+      <c r="D182" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="E180" s="19"/>
-      <c r="F180" s="18" t="s">
+      <c r="E182" s="19"/>
+      <c r="F182" s="18" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B181" s="19"/>
-      <c r="C181" s="19"/>
-      <c r="D181" s="19"/>
-      <c r="E181" s="19"/>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A182" s="11" t="s">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B183" s="19"/>
+      <c r="C183" s="19"/>
+      <c r="D183" s="19"/>
+      <c r="E183" s="19"/>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A184" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="B182" s="25" t="s">
+      <c r="B184" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="C182" s="25"/>
-      <c r="D182" s="25" t="s">
+      <c r="C184" s="25"/>
+      <c r="D184" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E182" s="35"/>
-      <c r="F182" s="25" t="s">
+      <c r="E184" s="35"/>
+      <c r="F184" s="25" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B183" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="C183" s="21"/>
-      <c r="D183" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E183" s="19"/>
-      <c r="F183" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B184" s="29" t="s">
-        <v>257</v>
-      </c>
-      <c r="C184" s="29"/>
-      <c r="D184" s="29" t="s">
-        <v>258</v>
-      </c>
-      <c r="E184" s="19"/>
-      <c r="F184" s="18" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B185" s="21" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="C185" s="21"/>
       <c r="D185" s="18" t="s">
@@ -5006,270 +5007,269 @@
       </c>
       <c r="E185" s="19"/>
       <c r="F185" s="18" t="s">
-        <v>228</v>
+        <v>156</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B186" s="29" t="s">
-        <v>351</v>
+        <v>257</v>
       </c>
       <c r="C186" s="29"/>
-      <c r="D186" s="29"/>
+      <c r="D186" s="29" t="s">
+        <v>258</v>
+      </c>
       <c r="E186" s="19"/>
-      <c r="F186" s="18"/>
+      <c r="F186" s="18" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B187" s="21" t="s">
-        <v>260</v>
+        <v>169</v>
       </c>
       <c r="C187" s="21"/>
       <c r="D187" s="18" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E187" s="19"/>
       <c r="F187" s="18" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B188" s="29" t="s">
+        <v>351</v>
+      </c>
+      <c r="C188" s="29"/>
+      <c r="D188" s="29"/>
+      <c r="E188" s="19"/>
+      <c r="F188" s="18"/>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B189" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="C189" s="21"/>
+      <c r="D189" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E189" s="19"/>
+      <c r="F189" s="18" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B188" s="21" t="s">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B190" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="C188" s="21"/>
-      <c r="D188" s="21" t="s">
+      <c r="C190" s="21"/>
+      <c r="D190" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="E188" s="19"/>
-      <c r="F188" s="18" t="s">
+      <c r="E190" s="19"/>
+      <c r="F190" s="18" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A190" s="11" t="s">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B191" s="23"/>
+      <c r="C191" s="23"/>
+      <c r="D191" s="23"/>
+      <c r="E191" s="19"/>
+      <c r="F191" s="19"/>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A192" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="B192" s="23"/>
+      <c r="C192" s="23"/>
+      <c r="D192" s="23"/>
+      <c r="E192" s="19"/>
+      <c r="F192" s="23" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A193" s="55"/>
+      <c r="B193" s="23"/>
+      <c r="C193" s="23"/>
+      <c r="D193" s="23"/>
+      <c r="E193" s="19"/>
+      <c r="F193" s="19"/>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A194" s="55"/>
+      <c r="B194" s="23"/>
+      <c r="C194" s="23"/>
+      <c r="D194" s="23"/>
+      <c r="E194" s="19"/>
+      <c r="F194" s="19"/>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A195" s="55"/>
+      <c r="B195" s="23"/>
+      <c r="C195" s="23"/>
+      <c r="D195" s="23"/>
+      <c r="E195" s="19"/>
+      <c r="F195" s="19"/>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A197" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="B190" s="25" t="s">
+      <c r="B197" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="C190" s="25"/>
-      <c r="D190" s="25" t="s">
+      <c r="C197" s="25"/>
+      <c r="D197" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E190" s="35"/>
-      <c r="F190" s="25" t="s">
+      <c r="E197" s="35"/>
+      <c r="F197" s="25" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B191" s="21" t="s">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B198" s="21" t="s">
         <v>226</v>
-      </c>
-      <c r="C191" s="21"/>
-      <c r="D191" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E191" s="23"/>
-      <c r="F191" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B192" s="21" t="s">
-        <v>230</v>
-      </c>
-      <c r="C192" s="21"/>
-      <c r="D192" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E192" s="23"/>
-      <c r="F192" s="18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B193" s="21"/>
-      <c r="C193" s="21"/>
-      <c r="D193" s="21"/>
-      <c r="E193" s="23"/>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A195" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B195" s="25" t="s">
-        <v>231</v>
-      </c>
-      <c r="C195" s="25"/>
-      <c r="D195" s="25"/>
-      <c r="E195" s="35"/>
-      <c r="F195" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B196" s="21" t="s">
-        <v>232</v>
-      </c>
-      <c r="C196" s="21"/>
-      <c r="D196" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E196" s="23"/>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B197" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="C197" s="21"/>
-      <c r="D197" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E197" s="23"/>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B198" s="21" t="s">
-        <v>234</v>
       </c>
       <c r="C198" s="21"/>
       <c r="D198" s="21" t="s">
         <v>47</v>
       </c>
       <c r="E198" s="23"/>
-      <c r="F198" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B199" s="29" t="s">
-        <v>235</v>
-      </c>
-      <c r="C199" s="29"/>
-      <c r="D199" s="29" t="s">
+      <c r="F198" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B199" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="C199" s="21"/>
+      <c r="D199" s="21" t="s">
         <v>47</v>
       </c>
       <c r="E199" s="23"/>
-      <c r="F199" s="17" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F199" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B200" s="21"/>
       <c r="C200" s="21"/>
       <c r="D200" s="21"/>
       <c r="E200" s="23"/>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B201" s="21"/>
-      <c r="C201" s="21"/>
-      <c r="D201" s="21"/>
-      <c r="E201" s="23"/>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B202" s="21"/>
-      <c r="C202" s="21"/>
-      <c r="D202" s="21"/>
-      <c r="E202" s="23"/>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A204" s="11" t="s">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A202" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B202" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="C202" s="25"/>
+      <c r="D202" s="25"/>
+      <c r="E202" s="35"/>
+      <c r="F202" s="17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B203" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="C203" s="21"/>
+      <c r="D203" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E203" s="23"/>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B204" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="C204" s="21"/>
+      <c r="D204" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E204" s="23"/>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B205" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="C205" s="21"/>
+      <c r="D205" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E205" s="23"/>
+      <c r="F205" s="17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B206" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="C206" s="29"/>
+      <c r="D206" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E206" s="23"/>
+      <c r="F206" s="17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B207" s="21"/>
+      <c r="C207" s="21"/>
+      <c r="D207" s="21"/>
+      <c r="E207" s="23"/>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B208" s="21"/>
+      <c r="C208" s="21"/>
+      <c r="D208" s="21"/>
+      <c r="E208" s="23"/>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B209" s="21"/>
+      <c r="C209" s="21"/>
+      <c r="D209" s="21"/>
+      <c r="E209" s="23"/>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A211" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B204" s="25"/>
-      <c r="C204" s="25"/>
-      <c r="D204" s="25"/>
-      <c r="E204" s="35"/>
-      <c r="I204" s="17" t="s">
+      <c r="B211" s="25"/>
+      <c r="C211" s="25"/>
+      <c r="D211" s="25"/>
+      <c r="E211" s="35"/>
+      <c r="I211" s="17" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B205" s="21"/>
-      <c r="C205" s="21"/>
-      <c r="D205" s="21"/>
-      <c r="E205" s="23"/>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B206" s="21"/>
-      <c r="C206" s="21"/>
-      <c r="D206" s="21"/>
-      <c r="E206" s="23"/>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A208" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B208" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="C208" s="25"/>
-      <c r="D208" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E208" s="35"/>
-      <c r="F208" s="17" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B209" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="C209" s="21"/>
-      <c r="D209" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E209" s="23"/>
-    </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B210" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="C210" s="21"/>
-      <c r="D210" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E210" s="23"/>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B211" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="C211" s="29"/>
-      <c r="D211" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="E211" s="24"/>
-    </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B212" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="C212" s="18"/>
-      <c r="D212" s="21" t="s">
-        <v>47</v>
-      </c>
+      <c r="B212" s="21"/>
+      <c r="C212" s="21"/>
+      <c r="D212" s="21"/>
       <c r="E212" s="23"/>
-      <c r="F212" s="17" t="s">
-        <v>148</v>
-      </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B213" s="21" t="s">
-        <v>177</v>
-      </c>
+      <c r="B213" s="21"/>
       <c r="C213" s="21"/>
-      <c r="D213" s="18"/>
-      <c r="E213" s="19"/>
-      <c r="F213" s="17" t="s">
-        <v>135</v>
-      </c>
+      <c r="D213" s="21"/>
+      <c r="E213" s="23"/>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A215" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B215" s="25" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C215" s="25"/>
       <c r="D215" s="25" t="s">
@@ -5279,23 +5279,20 @@
       <c r="F215" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="I215" s="23" t="s">
-        <v>149</v>
-      </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B216" s="21" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="C216" s="21"/>
       <c r="D216" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E216" s="23"/>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B217" s="21" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="C217" s="21"/>
       <c r="D217" s="21" t="s">
@@ -5339,20 +5336,26 @@
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A222" s="11" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B222" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C222" s="25"/>
       <c r="D222" s="25" t="s">
         <v>45</v>
       </c>
       <c r="E222" s="35"/>
+      <c r="F222" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="I222" s="23" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B223" s="21" t="s">
-        <v>238</v>
+        <v>203</v>
       </c>
       <c r="C223" s="21"/>
       <c r="D223" s="21" t="s">
@@ -5362,7 +5365,7 @@
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B224" s="21" t="s">
-        <v>169</v>
+        <v>204</v>
       </c>
       <c r="C224" s="21"/>
       <c r="D224" s="21" t="s">
@@ -5370,178 +5373,182 @@
       </c>
       <c r="E224" s="23"/>
     </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B225" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="C225" s="29"/>
+      <c r="D225" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="E225" s="24"/>
+    </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A226" s="17"/>
-      <c r="B226" s="40" t="s">
+      <c r="B226" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="C226" s="18"/>
+      <c r="D226" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E226" s="23"/>
+      <c r="F226" s="17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B227" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C227" s="21"/>
+      <c r="D227" s="18"/>
+      <c r="E227" s="19"/>
+      <c r="F227" s="17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A229" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B229" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="C226" s="40"/>
-      <c r="D226" s="40" t="s">
+      <c r="C229" s="25"/>
+      <c r="D229" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E229" s="35"/>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B230" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="E226" s="40"/>
-      <c r="F226" s="40" t="s">
+      <c r="C230" s="21"/>
+      <c r="D230" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E230" s="23"/>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B231" s="21" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="227" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A227" s="17"/>
-      <c r="B227" s="41">
+      <c r="C231" s="21"/>
+      <c r="D231" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E231" s="23"/>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A233" s="17"/>
+      <c r="B233" s="40" t="s">
+        <v>241</v>
+      </c>
+      <c r="C233" s="40"/>
+      <c r="D233" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="E233" s="40"/>
+      <c r="F233" s="40" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A234" s="17"/>
+      <c r="B234" s="41">
         <v>1</v>
       </c>
-      <c r="C227" s="41"/>
-      <c r="D227" s="42" t="s">
+      <c r="C234" s="41"/>
+      <c r="D234" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="E227" s="42"/>
-      <c r="F227" s="42" t="s">
+      <c r="E234" s="42"/>
+      <c r="F234" s="42" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A228" s="17"/>
-      <c r="B228" s="41">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A235" s="17"/>
+      <c r="B235" s="41">
         <v>2</v>
       </c>
-      <c r="C228" s="41"/>
-      <c r="D228" s="42" t="s">
+      <c r="C235" s="41"/>
+      <c r="D235" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="E228" s="42"/>
-      <c r="F228" s="42" t="s">
+      <c r="E235" s="42"/>
+      <c r="F235" s="42" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="229" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A229" s="17"/>
-      <c r="B229" s="41">
+    <row r="236" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A236" s="17"/>
+      <c r="B236" s="41">
         <v>3</v>
       </c>
-      <c r="C229" s="41"/>
-      <c r="D229" s="42" t="s">
+      <c r="C236" s="41"/>
+      <c r="D236" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="E229" s="42"/>
-      <c r="F229" s="42" t="s">
+      <c r="E236" s="42"/>
+      <c r="F236" s="42" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A230" s="17"/>
-      <c r="B230" s="41">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A237" s="17"/>
+      <c r="B237" s="41">
         <v>4</v>
       </c>
-      <c r="C230" s="41"/>
-      <c r="D230" s="42" t="s">
+      <c r="C237" s="41"/>
+      <c r="D237" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="E230" s="42"/>
-      <c r="F230" s="42" t="s">
+      <c r="E237" s="42"/>
+      <c r="F237" s="42" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A231" s="17"/>
-      <c r="B231" s="41">
+    <row r="238" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A238" s="17"/>
+      <c r="B238" s="41">
         <v>5</v>
       </c>
-      <c r="C231" s="41"/>
-      <c r="D231" s="42" t="s">
+      <c r="C238" s="41"/>
+      <c r="D238" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="E231" s="42"/>
-      <c r="F231" s="42" t="s">
+      <c r="E238" s="42"/>
+      <c r="F238" s="42" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A232" s="17"/>
-      <c r="B232" s="41">
+    <row r="239" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A239" s="17"/>
+      <c r="B239" s="41">
         <v>6</v>
       </c>
-      <c r="C232" s="41"/>
-      <c r="D232" s="42" t="s">
+      <c r="C239" s="41"/>
+      <c r="D239" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="E232" s="42"/>
-      <c r="F232" s="42" t="s">
+      <c r="E239" s="42"/>
+      <c r="F239" s="42" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A234" s="11" t="s">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A241" s="11" t="s">
         <v>352</v>
       </c>
-      <c r="B234" s="65"/>
-      <c r="C234" s="65"/>
-      <c r="D234" s="65"/>
-    </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B235" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="C235" s="18"/>
-      <c r="D235" s="18"/>
-      <c r="E235" s="18"/>
-      <c r="F235" s="18"/>
-    </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B236" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="C236" s="18"/>
-      <c r="D236" s="18"/>
-      <c r="E236" s="18"/>
-      <c r="F236" s="18"/>
-    </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B237" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="C237" s="18"/>
-      <c r="D237" s="18"/>
-      <c r="E237" s="18"/>
-      <c r="F237" s="18"/>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B238" s="21" t="s">
-        <v>353</v>
-      </c>
-      <c r="C238" s="18"/>
-      <c r="D238" s="18"/>
-      <c r="E238" s="18"/>
-      <c r="F238" s="18"/>
-    </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B239" s="21" t="s">
-        <v>354</v>
-      </c>
-      <c r="C239" s="18"/>
-      <c r="D239" s="18"/>
-      <c r="E239" s="18"/>
-      <c r="F239" s="18"/>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B240" s="21" t="s">
-        <v>355</v>
-      </c>
-      <c r="C240" s="18"/>
-      <c r="D240" s="18"/>
-      <c r="E240" s="18"/>
-      <c r="F240" s="18"/>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B241" s="21" t="s">
-        <v>356</v>
-      </c>
-      <c r="C241" s="18"/>
-      <c r="D241" s="18"/>
-      <c r="E241" s="18"/>
-      <c r="F241" s="18"/>
+      <c r="B241" s="65"/>
+      <c r="C241" s="65"/>
+      <c r="D241" s="65"/>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B242" s="21" t="s">
-        <v>357</v>
+        <v>187</v>
       </c>
       <c r="C242" s="18"/>
       <c r="D242" s="18"/>
@@ -5550,7 +5557,7 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B243" s="21" t="s">
-        <v>358</v>
+        <v>203</v>
       </c>
       <c r="C243" s="18"/>
       <c r="D243" s="18"/>
@@ -5559,237 +5566,223 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B244" s="21" t="s">
-        <v>247</v>
+        <v>168</v>
       </c>
       <c r="C244" s="18"/>
       <c r="D244" s="18"/>
       <c r="E244" s="18"/>
       <c r="F244" s="18"/>
     </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B245" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="C245" s="18"/>
+      <c r="D245" s="18"/>
+      <c r="E245" s="18"/>
+      <c r="F245" s="18"/>
+    </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A246" s="11" t="s">
+      <c r="B246" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="C246" s="18"/>
+      <c r="D246" s="18"/>
+      <c r="E246" s="18"/>
+      <c r="F246" s="18"/>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B247" s="21" t="s">
+        <v>355</v>
+      </c>
+      <c r="C247" s="18"/>
+      <c r="D247" s="18"/>
+      <c r="E247" s="18"/>
+      <c r="F247" s="18"/>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B248" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="C248" s="18"/>
+      <c r="D248" s="18"/>
+      <c r="E248" s="18"/>
+      <c r="F248" s="18"/>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B249" s="21" t="s">
+        <v>357</v>
+      </c>
+      <c r="C249" s="18"/>
+      <c r="D249" s="18"/>
+      <c r="E249" s="18"/>
+      <c r="F249" s="18"/>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B250" s="21" t="s">
+        <v>358</v>
+      </c>
+      <c r="C250" s="18"/>
+      <c r="D250" s="18"/>
+      <c r="E250" s="18"/>
+      <c r="F250" s="18"/>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B251" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="C251" s="18"/>
+      <c r="D251" s="18"/>
+      <c r="E251" s="18"/>
+      <c r="F251" s="18"/>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A253" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="B246" s="25"/>
-      <c r="C246" s="25"/>
-      <c r="D246" s="25"/>
-      <c r="F246" s="17" t="s">
+      <c r="B253" s="25"/>
+      <c r="C253" s="25"/>
+      <c r="D253" s="25"/>
+      <c r="F253" s="17" t="s">
         <v>451</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B247" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="D247" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F247" s="17" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A248" s="72"/>
-      <c r="B248" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="D248" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="F248" s="36" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B249" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="D249" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F249" s="23" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B250" s="17" t="s">
-        <v>392</v>
-      </c>
-      <c r="D250" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F250" s="17" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B251" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="D251" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F251" s="17" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B252" s="17" t="s">
-        <v>369</v>
-      </c>
-      <c r="D252" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F252" s="17" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B253" s="17" t="s">
-        <v>370</v>
-      </c>
-      <c r="D253" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F253" s="17" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B254" s="17" t="s">
-        <v>396</v>
+        <v>187</v>
       </c>
       <c r="D254" s="17" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="F254" s="17" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B255" s="17" t="s">
-        <v>440</v>
-      </c>
-      <c r="D255" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F255" s="17" t="s">
-        <v>452</v>
+        <v>412</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A255" s="67"/>
+      <c r="B255" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="D255" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F255" s="36" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B256" s="17" t="s">
-        <v>402</v>
+        <v>247</v>
       </c>
       <c r="D256" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F256" s="17" t="s">
-        <v>423</v>
+        <v>60</v>
+      </c>
+      <c r="F256" s="23" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="257" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B257" s="17" t="s">
-        <v>413</v>
+        <v>392</v>
       </c>
       <c r="D257" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F257" s="17" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="258" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B258" s="17" t="s">
-        <v>414</v>
+        <v>393</v>
       </c>
       <c r="D258" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F258" s="17" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
     </row>
     <row r="259" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B259" s="17" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D259" s="17" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="F259" s="17" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="260" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B260" s="17" t="s">
-        <v>372</v>
-      </c>
-      <c r="D260" s="17" t="s">
-        <v>47</v>
+        <v>370</v>
+      </c>
+      <c r="D260" s="23" t="s">
+        <v>60</v>
       </c>
       <c r="F260" s="17" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="261" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B261" s="17" t="s">
-        <v>375</v>
+        <v>396</v>
       </c>
       <c r="D261" s="17" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="F261" s="17" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="262" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B262" s="17" t="s">
-        <v>376</v>
-      </c>
-      <c r="D262" s="17" t="s">
-        <v>47</v>
+        <v>440</v>
+      </c>
+      <c r="D262" s="23" t="s">
+        <v>45</v>
       </c>
       <c r="F262" s="17" t="s">
-        <v>421</v>
+        <v>452</v>
       </c>
     </row>
     <row r="263" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B263" s="17" t="s">
-        <v>379</v>
+        <v>402</v>
       </c>
       <c r="D263" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F263" s="17" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="264" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B264" s="17" t="s">
-        <v>380</v>
+        <v>413</v>
       </c>
       <c r="D264" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F264" s="17" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="265" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B265" s="17" t="s">
-        <v>381</v>
+        <v>414</v>
       </c>
       <c r="D265" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F265" s="17" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="266" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B266" s="17" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="D266" s="17" t="s">
         <v>47</v>
@@ -5800,7 +5793,7 @@
     </row>
     <row r="267" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B267" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D267" s="17" t="s">
         <v>47</v>
@@ -5811,7 +5804,7 @@
     </row>
     <row r="268" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B268" s="17" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D268" s="17" t="s">
         <v>47</v>
@@ -5822,7 +5815,7 @@
     </row>
     <row r="269" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B269" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D269" s="17" t="s">
         <v>47</v>
@@ -5833,7 +5826,7 @@
     </row>
     <row r="270" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B270" s="17" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D270" s="17" t="s">
         <v>47</v>
@@ -5844,7 +5837,7 @@
     </row>
     <row r="271" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B271" s="17" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D271" s="17" t="s">
         <v>47</v>
@@ -5855,7 +5848,7 @@
     </row>
     <row r="272" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B272" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D272" s="17" t="s">
         <v>47</v>
@@ -5864,9 +5857,9 @@
         <v>421</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="273" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B273" s="17" t="s">
-        <v>420</v>
+        <v>389</v>
       </c>
       <c r="D273" s="17" t="s">
         <v>47</v>
@@ -5875,9 +5868,9 @@
         <v>421</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="274" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B274" s="17" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="D274" s="17" t="s">
         <v>47</v>
@@ -5886,394 +5879,387 @@
         <v>421</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="275" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B275" s="17" t="s">
+        <v>374</v>
+      </c>
+      <c r="D275" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F275" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="276" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B276" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="D276" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F276" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="277" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B277" s="17" t="s">
+        <v>378</v>
+      </c>
+      <c r="D277" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F277" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="278" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B278" s="17" t="s">
+        <v>383</v>
+      </c>
+      <c r="D278" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F278" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="279" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B279" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="D279" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F279" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="280" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B280" s="17" t="s">
+        <v>420</v>
+      </c>
+      <c r="D280" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F280" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="281" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B281" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="D281" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F281" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="282" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B282" s="17" t="s">
         <v>384</v>
       </c>
-      <c r="D275" s="17" t="s">
+      <c r="D282" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F275" s="17" t="s">
+      <c r="F282" s="17" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B276" s="17" t="s">
+    <row r="283" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B283" s="17" t="s">
         <v>385</v>
       </c>
-      <c r="D276" s="17" t="s">
+      <c r="D283" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F276" s="17" t="s">
+      <c r="F283" s="17" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B277" s="17" t="s">
+    <row r="284" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B284" s="17" t="s">
         <v>386</v>
       </c>
-      <c r="D277" s="17" t="s">
+      <c r="D284" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F277" s="17" t="s">
+      <c r="F284" s="17" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B278" s="17" t="s">
+    <row r="285" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B285" s="17" t="s">
         <v>388</v>
       </c>
-      <c r="D278" s="17" t="s">
+      <c r="D285" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F278" s="17" t="s">
+      <c r="F285" s="17" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B279" s="17" t="s">
+    <row r="286" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B286" s="17" t="s">
         <v>395</v>
       </c>
-      <c r="D279" s="17" t="s">
+      <c r="D286" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F279" s="17" t="s">
+      <c r="F286" s="17" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B280" s="17" t="s">
+    <row r="287" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B287" s="17" t="s">
         <v>390</v>
       </c>
-      <c r="D280" s="17" t="s">
+      <c r="D287" s="17" t="s">
         <v>407</v>
       </c>
-      <c r="F280" s="17" t="s">
+      <c r="F287" s="17" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B281" s="17" t="s">
+    <row r="288" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B288" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="D281" s="17" t="s">
+      <c r="D288" s="17" t="s">
         <v>407</v>
       </c>
-      <c r="F281" s="17" t="s">
+      <c r="F288" s="17" t="s">
         <v>424</v>
-      </c>
-    </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B282" s="17" t="s">
-        <v>404</v>
-      </c>
-      <c r="D282" s="17" t="s">
-        <v>407</v>
-      </c>
-      <c r="F282" s="17" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B283" s="17" t="s">
-        <v>391</v>
-      </c>
-      <c r="D283" s="17" t="s">
-        <v>407</v>
-      </c>
-      <c r="F283" s="17" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B284" s="17" t="s">
-        <v>405</v>
-      </c>
-      <c r="D284" s="17" t="s">
-        <v>407</v>
-      </c>
-      <c r="F284" s="17" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B285" s="17" t="s">
-        <v>394</v>
-      </c>
-      <c r="D285" s="17" t="s">
-        <v>407</v>
-      </c>
-      <c r="F285" s="17" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A287" s="11" t="s">
-        <v>441</v>
-      </c>
-      <c r="B287" s="25"/>
-      <c r="C287" s="25"/>
-      <c r="D287" s="25"/>
-      <c r="F287" s="17" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B288" s="17" t="s">
-        <v>434</v>
-      </c>
-      <c r="D288" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F288" s="17" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B289" s="17" t="s">
-        <v>435</v>
-      </c>
-      <c r="D289" s="23" t="s">
-        <v>47</v>
+        <v>404</v>
+      </c>
+      <c r="D289" s="17" t="s">
+        <v>407</v>
       </c>
       <c r="F289" s="17" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B290" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="D290" s="23" t="s">
-        <v>45</v>
+        <v>391</v>
+      </c>
+      <c r="D290" s="17" t="s">
+        <v>407</v>
       </c>
       <c r="F290" s="17" t="s">
-        <v>412</v>
+        <v>427</v>
       </c>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B291" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="D291" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F291" s="36" t="s">
-        <v>411</v>
+        <v>405</v>
+      </c>
+      <c r="D291" s="17" t="s">
+        <v>407</v>
+      </c>
+      <c r="F291" s="17" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B292" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="D292" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F292" s="23" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B293" s="17" t="s">
-        <v>436</v>
-      </c>
-      <c r="D293" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F293" s="23" t="s">
-        <v>462</v>
+        <v>394</v>
+      </c>
+      <c r="D292" s="17" t="s">
+        <v>407</v>
+      </c>
+      <c r="F292" s="17" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B294" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="D294" s="23" t="s">
-        <v>45</v>
-      </c>
+      <c r="A294" s="11" t="s">
+        <v>441</v>
+      </c>
+      <c r="B294" s="25"/>
+      <c r="C294" s="25"/>
+      <c r="D294" s="25"/>
       <c r="F294" s="17" t="s">
-        <v>457</v>
+        <v>422</v>
       </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B295" s="17" t="s">
-        <v>369</v>
+        <v>434</v>
       </c>
       <c r="D295" s="23" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="F295" s="17" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B296" s="17" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D296" s="23" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F296" s="17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B297" s="17" t="s">
-        <v>438</v>
+        <v>187</v>
       </c>
       <c r="D297" s="23" t="s">
         <v>45</v>
       </c>
       <c r="F297" s="17" t="s">
-        <v>461</v>
+        <v>412</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B298" s="17" t="s">
-        <v>439</v>
+        <v>203</v>
       </c>
       <c r="D298" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F298" s="17" t="s">
-        <v>459</v>
+        <v>47</v>
+      </c>
+      <c r="F298" s="36" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B299" s="17" t="s">
-        <v>440</v>
+        <v>247</v>
       </c>
       <c r="D299" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F299" s="17" t="s">
-        <v>452</v>
+        <v>60</v>
+      </c>
+      <c r="F299" s="23" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A300" s="17"/>
       <c r="B300" s="17" t="s">
-        <v>402</v>
+        <v>436</v>
       </c>
       <c r="D300" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F300" s="17" t="s">
-        <v>423</v>
+        <v>60</v>
+      </c>
+      <c r="F300" s="23" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A301" s="17"/>
       <c r="B301" s="17" t="s">
-        <v>413</v>
+        <v>223</v>
       </c>
       <c r="D301" s="23" t="s">
         <v>45</v>
       </c>
       <c r="F301" s="17" t="s">
-        <v>415</v>
+        <v>457</v>
       </c>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A302" s="17"/>
       <c r="B302" s="17" t="s">
-        <v>414</v>
+        <v>369</v>
       </c>
       <c r="D302" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F302" s="17" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B303" s="17" t="s">
+        <v>437</v>
+      </c>
+      <c r="D303" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F302" s="17" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A303" s="17"/>
-      <c r="B303" s="17" t="s">
-        <v>371</v>
-      </c>
-      <c r="D303" s="23" t="s">
-        <v>47</v>
-      </c>
       <c r="F303" s="17" t="s">
-        <v>421</v>
+        <v>460</v>
       </c>
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A304" s="17"/>
       <c r="B304" s="17" t="s">
-        <v>372</v>
+        <v>438</v>
       </c>
       <c r="D304" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F304" s="17" t="s">
-        <v>421</v>
+        <v>461</v>
       </c>
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A305" s="17"/>
       <c r="B305" s="17" t="s">
-        <v>375</v>
+        <v>439</v>
       </c>
       <c r="D305" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F305" s="17" t="s">
-        <v>421</v>
+        <v>459</v>
       </c>
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A306" s="17"/>
       <c r="B306" s="17" t="s">
-        <v>376</v>
+        <v>440</v>
       </c>
       <c r="D306" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F306" s="17" t="s">
-        <v>421</v>
+        <v>452</v>
       </c>
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A307" s="17"/>
       <c r="B307" s="17" t="s">
-        <v>379</v>
+        <v>402</v>
       </c>
       <c r="D307" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F307" s="17" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A308" s="17"/>
       <c r="B308" s="17" t="s">
-        <v>380</v>
+        <v>413</v>
       </c>
       <c r="D308" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F308" s="17" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A309" s="17"/>
       <c r="B309" s="17" t="s">
-        <v>381</v>
+        <v>414</v>
       </c>
       <c r="D309" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F309" s="17" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A310" s="17"/>
       <c r="B310" s="17" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="D310" s="23" t="s">
         <v>47</v>
@@ -6285,7 +6271,7 @@
     <row r="311" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A311" s="17"/>
       <c r="B311" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D311" s="23" t="s">
         <v>47</v>
@@ -6297,7 +6283,7 @@
     <row r="312" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A312" s="17"/>
       <c r="B312" s="17" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D312" s="23" t="s">
         <v>47</v>
@@ -6309,7 +6295,7 @@
     <row r="313" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A313" s="17"/>
       <c r="B313" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D313" s="23" t="s">
         <v>47</v>
@@ -6321,7 +6307,7 @@
     <row r="314" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A314" s="17"/>
       <c r="B314" s="17" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D314" s="23" t="s">
         <v>47</v>
@@ -6333,7 +6319,7 @@
     <row r="315" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A315" s="17"/>
       <c r="B315" s="17" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D315" s="23" t="s">
         <v>47</v>
@@ -6345,7 +6331,7 @@
     <row r="316" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A316" s="17"/>
       <c r="B316" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D316" s="23" t="s">
         <v>47</v>
@@ -6357,7 +6343,7 @@
     <row r="317" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A317" s="17"/>
       <c r="B317" s="17" t="s">
-        <v>420</v>
+        <v>389</v>
       </c>
       <c r="D317" s="23" t="s">
         <v>47</v>
@@ -6369,7 +6355,7 @@
     <row r="318" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A318" s="17"/>
       <c r="B318" s="17" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="D318" s="23" t="s">
         <v>47</v>
@@ -6381,264 +6367,404 @@
     <row r="319" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A319" s="17"/>
       <c r="B319" s="17" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="D319" s="23" t="s">
         <v>47</v>
       </c>
       <c r="F319" s="17" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A320" s="17"/>
       <c r="B320" s="17" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D320" s="23" t="s">
         <v>47</v>
       </c>
       <c r="F320" s="17" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A321" s="17"/>
       <c r="B321" s="17" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="D321" s="23" t="s">
         <v>47</v>
       </c>
       <c r="F321" s="17" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A322" s="17"/>
       <c r="B322" s="17" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="D322" s="23" t="s">
         <v>47</v>
       </c>
       <c r="F322" s="17" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
     </row>
     <row r="323" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A323" s="17"/>
       <c r="B323" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="D323" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F323" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A324" s="17"/>
+      <c r="B324" s="17" t="s">
+        <v>420</v>
+      </c>
+      <c r="D324" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F324" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A325" s="17"/>
+      <c r="B325" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="D325" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F325" s="17" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A326" s="17"/>
+      <c r="B326" s="17" t="s">
+        <v>384</v>
+      </c>
+      <c r="D326" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F326" s="17" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A327" s="17"/>
+      <c r="B327" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="D327" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F327" s="17" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A328" s="17"/>
+      <c r="B328" s="17" t="s">
+        <v>386</v>
+      </c>
+      <c r="D328" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F328" s="17" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A329" s="17"/>
+      <c r="B329" s="17" t="s">
+        <v>388</v>
+      </c>
+      <c r="D329" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F329" s="17" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A330" s="17"/>
+      <c r="B330" s="17" t="s">
         <v>395</v>
       </c>
-      <c r="D323" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F323" s="17" t="s">
+      <c r="D330" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F330" s="17" t="s">
         <v>433</v>
-      </c>
-    </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B324" s="17" t="s">
-        <v>390</v>
-      </c>
-      <c r="D324" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F324" s="17" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B325" s="17" t="s">
-        <v>403</v>
-      </c>
-      <c r="D325" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F325" s="17" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B326" s="17" t="s">
-        <v>404</v>
-      </c>
-      <c r="D326" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F326" s="17" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B327" s="17" t="s">
-        <v>391</v>
-      </c>
-      <c r="D327" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F327" s="17" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B328" s="17" t="s">
-        <v>394</v>
-      </c>
-      <c r="D328" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F328" s="17" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A330" s="11" t="s">
-        <v>449</v>
-      </c>
-      <c r="B330" s="25"/>
-      <c r="C330" s="25"/>
-      <c r="D330" s="25"/>
-      <c r="F330" s="17" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B331" s="17" t="s">
-        <v>434</v>
+        <v>390</v>
+      </c>
+      <c r="D331" s="23" t="s">
+        <v>47</v>
       </c>
       <c r="F331" s="17" t="s">
-        <v>453</v>
+        <v>425</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B332" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="F332" s="23" t="s">
-        <v>456</v>
+        <v>403</v>
+      </c>
+      <c r="D332" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F332" s="17" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B333" s="17" t="s">
-        <v>442</v>
-      </c>
-      <c r="F333" s="23" t="s">
-        <v>463</v>
+        <v>404</v>
+      </c>
+      <c r="D333" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F333" s="17" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B334" s="17" t="s">
-        <v>392</v>
-      </c>
-      <c r="F334" s="23" t="s">
-        <v>464</v>
+        <v>391</v>
+      </c>
+      <c r="D334" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F334" s="17" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B335" s="17" t="s">
+        <v>394</v>
+      </c>
+      <c r="D335" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F335" s="17" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A337" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="B337" s="25"/>
+      <c r="C337" s="25"/>
+      <c r="D337" s="25"/>
+      <c r="F337" s="17" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B338" s="17" t="s">
+        <v>434</v>
+      </c>
+      <c r="D338" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F338" s="17" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B339" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="D339" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F339" s="23" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B340" s="17" t="s">
+        <v>442</v>
+      </c>
+      <c r="D340" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F340" s="23" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B341" s="17" t="s">
+        <v>392</v>
+      </c>
+      <c r="D341" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F341" s="23" t="s">
+        <v>464</v>
+      </c>
+      <c r="G341" s="23"/>
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B342" s="17" t="s">
         <v>393</v>
       </c>
-      <c r="F335" s="23" t="s">
+      <c r="D342" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F342" s="23" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B336" s="17" t="s">
+      <c r="G342" s="23"/>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B343" s="17" t="s">
         <v>443</v>
       </c>
-      <c r="F336" s="23" t="s">
+      <c r="D343" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F343" s="23" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="337" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B337" s="17" t="s">
+      <c r="G343" s="23"/>
+    </row>
+    <row r="344" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B344" s="17" t="s">
         <v>444</v>
       </c>
-      <c r="F337" s="23" t="s">
+      <c r="D344" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F344" s="23" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="338" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B338" s="17" t="s">
+      <c r="G344" s="23"/>
+    </row>
+    <row r="345" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B345" s="17" t="s">
         <v>445</v>
       </c>
-      <c r="F338" s="23" t="s">
+      <c r="D345" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F345" s="23" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="339" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B339" s="17" t="s">
+      <c r="G345" s="23"/>
+    </row>
+    <row r="346" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B346" s="17" t="s">
         <v>446</v>
       </c>
-      <c r="F339" s="23" t="s">
+      <c r="D346" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F346" s="23" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="340" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B340" s="17" t="s">
+      <c r="G346" s="23"/>
+    </row>
+    <row r="347" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B347" s="17" t="s">
         <v>447</v>
       </c>
-      <c r="F340" s="23" t="s">
+      <c r="D347" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F347" s="23" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="341" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B341" s="17" t="s">
+      <c r="G347" s="23"/>
+    </row>
+    <row r="348" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B348" s="17" t="s">
         <v>448</v>
       </c>
-      <c r="F341" s="23" t="s">
+      <c r="D348" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F348" s="23" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="342" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B342" s="17" t="s">
+      <c r="G348" s="23"/>
+    </row>
+    <row r="349" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B349" s="17" t="s">
         <v>390</v>
       </c>
-      <c r="F342" s="17" t="s">
+      <c r="D349" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F349" s="17" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="343" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B343" s="17" t="s">
+    <row r="350" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B350" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="F343" s="17" t="s">
+      <c r="D350" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F350" s="17" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="344" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B344" s="17" t="s">
+    <row r="351" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B351" s="17" t="s">
         <v>404</v>
       </c>
-      <c r="F344" s="17" t="s">
+      <c r="D351" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F351" s="17" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="345" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B345" s="17" t="s">
+    <row r="352" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B352" s="17" t="s">
         <v>391</v>
       </c>
-      <c r="F345" s="17" t="s">
+      <c r="D352" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F352" s="17" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="346" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B346" s="17" t="s">
+    <row r="353" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B353" s="17" t="s">
         <v>394</v>
       </c>
-      <c r="F346" s="17" t="s">
+      <c r="D353" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F353" s="17" t="s">
         <v>408</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="I124:I136"/>
+    <mergeCell ref="I126:I138"/>
     <mergeCell ref="F42:H42"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J140" r:id="rId1" xr:uid="{C542003A-DE46-4D98-A11B-9CC195E7F11A}"/>
+    <hyperlink ref="J142" r:id="rId1" xr:uid="{C542003A-DE46-4D98-A11B-9CC195E7F11A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="90" r:id="rId2"/>
@@ -6650,8 +6776,8 @@
   <dimension ref="A1:N240"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B156" sqref="B156"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>

</xml_diff>